<commit_message>
Rewritten tokenization exceptions handling
</commit_message>
<xml_diff>
--- a/docs/SemTi-Kamols_morphotags.xlsx
+++ b/docs/SemTi-Kamols_morphotags.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="545">
   <si>
     <t>Latviešu valodas morfoloģisko pazīmju kopa</t>
   </si>
@@ -6216,9 +6216,6 @@
     </r>
   </si>
   <si>
-    <t>daudzskaitlis</t>
-  </si>
-  <si>
     <t>ģenitīvs (vienīgā forma)</t>
   </si>
   <si>
@@ -6561,6 +6558,18 @@
   </si>
   <si>
     <t>Latvija, Vidusāzija</t>
+  </si>
+  <si>
+    <t>abi, abas, viss, visa, pats, katra, ikkatra, ikviens</t>
+  </si>
+  <si>
+    <t>tas, tā, šāds, tāda, viņa (viņā saulē)</t>
+  </si>
+  <si>
+    <t>vsk. nominatīvs, izņemot daudzkskaitliniekus, kuriem tezaurā ir norāde, ka tikai daudzskaitlī, un mēs par to piekrītam</t>
+  </si>
+  <si>
+    <t>daudzskaitlis, ja vsk. forma vispār netiek lietota</t>
   </si>
 </sst>
 </file>
@@ -8617,10 +8626,10 @@
         <v>434</v>
       </c>
       <c r="E5" s="40" t="s">
+        <v>532</v>
+      </c>
+      <c r="F5" s="27" t="s">
         <v>533</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -8679,7 +8688,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8690,7 +8699,7 @@
     <col min="4" max="4" width="32.1640625" style="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.33203125" style="28" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.6640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" style="28" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" style="26" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" style="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="53" style="26" bestFit="1" customWidth="1"/>
@@ -8716,7 +8725,7 @@
       <c r="F1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="37" t="s">
         <v>487</v>
       </c>
       <c r="H1" s="20" t="s">
@@ -8729,7 +8738,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="22" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="22" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A2" s="43">
         <v>1</v>
       </c>
@@ -8744,10 +8753,10 @@
       </c>
       <c r="E2" s="39"/>
       <c r="F2" s="39" t="s">
-        <v>535</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>488</v>
+        <v>534</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>543</v>
       </c>
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
@@ -8764,7 +8773,7 @@
       <c r="D3" s="23"/>
       <c r="E3" s="39"/>
       <c r="F3" s="39"/>
-      <c r="G3" s="23"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
@@ -8783,7 +8792,7 @@
       <c r="F4" s="40" t="s">
         <v>514</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="40" t="s">
         <v>489</v>
       </c>
       <c r="H4" s="27" t="s">
@@ -8804,9 +8813,9 @@
       </c>
       <c r="E5" s="40"/>
       <c r="F5" s="40" t="s">
-        <v>541</v>
-      </c>
-      <c r="G5" s="27" t="s">
+        <v>540</v>
+      </c>
+      <c r="G5" s="40" t="s">
         <v>490</v>
       </c>
       <c r="H5" s="27" t="s">
@@ -8828,7 +8837,7 @@
       <c r="D6" s="23"/>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
-      <c r="G6" s="23"/>
+      <c r="G6" s="39"/>
       <c r="H6" s="23" t="s">
         <v>32</v>
       </c>
@@ -8851,7 +8860,7 @@
       <c r="F7" s="40" t="s">
         <v>442</v>
       </c>
-      <c r="G7" s="27"/>
+      <c r="G7" s="40"/>
       <c r="H7" s="27" t="s">
         <v>34</v>
       </c>
@@ -8872,7 +8881,7 @@
       <c r="F8" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="27"/>
+      <c r="G8" s="40"/>
       <c r="H8" s="27" t="s">
         <v>35</v>
       </c>
@@ -8895,7 +8904,7 @@
       <c r="F9" s="40" t="s">
         <v>471</v>
       </c>
-      <c r="G9" s="27"/>
+      <c r="G9" s="40"/>
       <c r="H9" s="71"/>
       <c r="I9" s="71"/>
       <c r="J9" s="27"/>
@@ -8914,7 +8923,7 @@
       <c r="F10" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="30"/>
+      <c r="G10" s="48"/>
       <c r="H10" s="30" t="s">
         <v>38</v>
       </c>
@@ -8936,7 +8945,7 @@
       <c r="D11" s="23"/>
       <c r="E11" s="39"/>
       <c r="F11" s="39"/>
-      <c r="G11" s="23"/>
+      <c r="G11" s="39"/>
       <c r="H11" s="23" t="s">
         <v>41</v>
       </c>
@@ -8955,7 +8964,7 @@
       </c>
       <c r="E12" s="40"/>
       <c r="F12" s="40"/>
-      <c r="G12" s="27"/>
+      <c r="G12" s="40"/>
       <c r="H12" s="27" t="s">
         <v>43</v>
       </c>
@@ -8974,7 +8983,7 @@
       </c>
       <c r="E13" s="40"/>
       <c r="F13" s="40"/>
-      <c r="G13" s="27"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="27" t="s">
         <v>45</v>
       </c>
@@ -8997,14 +9006,14 @@
       <c r="F14" s="40" t="s">
         <v>516</v>
       </c>
-      <c r="G14" s="27"/>
+      <c r="G14" s="40"/>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
       <c r="J14" s="27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B15" s="27"/>
       <c r="C15" s="27" t="s">
         <v>46</v>
@@ -9018,8 +9027,8 @@
       <c r="F15" s="40" t="s">
         <v>515</v>
       </c>
-      <c r="G15" s="27" t="s">
-        <v>520</v>
+      <c r="G15" s="40" t="s">
+        <v>544</v>
       </c>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
@@ -9041,7 +9050,7 @@
       <c r="F16" s="40" t="s">
         <v>472</v>
       </c>
-      <c r="G16" s="27"/>
+      <c r="G16" s="40"/>
       <c r="H16" s="27"/>
       <c r="I16" s="27"/>
       <c r="J16" s="27"/>
@@ -9057,7 +9066,7 @@
       <c r="D17" s="23"/>
       <c r="E17" s="39"/>
       <c r="F17" s="39"/>
-      <c r="G17" s="23"/>
+      <c r="G17" s="39"/>
       <c r="H17" s="23" t="s">
         <v>48</v>
       </c>
@@ -9078,7 +9087,7 @@
       <c r="F18" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="27"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="27" t="s">
         <v>50</v>
       </c>
@@ -9099,7 +9108,7 @@
       <c r="F19" s="40" t="s">
         <v>465</v>
       </c>
-      <c r="G19" s="27"/>
+      <c r="G19" s="40"/>
       <c r="H19" s="27" t="s">
         <v>52</v>
       </c>
@@ -9120,7 +9129,7 @@
       <c r="F20" s="40" t="s">
         <v>466</v>
       </c>
-      <c r="G20" s="27"/>
+      <c r="G20" s="40"/>
       <c r="H20" s="27" t="s">
         <v>54</v>
       </c>
@@ -9141,7 +9150,7 @@
       <c r="F21" s="40" t="s">
         <v>467</v>
       </c>
-      <c r="G21" s="27"/>
+      <c r="G21" s="40"/>
       <c r="H21" s="27" t="s">
         <v>56</v>
       </c>
@@ -9162,7 +9171,7 @@
       <c r="F22" s="40" t="s">
         <v>468</v>
       </c>
-      <c r="G22" s="27"/>
+      <c r="G22" s="40"/>
       <c r="H22" s="27" t="s">
         <v>58</v>
       </c>
@@ -9183,7 +9192,7 @@
       <c r="F23" s="40" t="s">
         <v>469</v>
       </c>
-      <c r="G23" s="27"/>
+      <c r="G23" s="40"/>
       <c r="H23" s="27" t="s">
         <v>60</v>
       </c>
@@ -9206,7 +9215,7 @@
       <c r="F24" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="30"/>
+      <c r="G24" s="48"/>
       <c r="H24" s="30"/>
       <c r="I24" s="30"/>
       <c r="J24" s="30" t="s">
@@ -9227,7 +9236,7 @@
       <c r="F25" s="40" t="s">
         <v>473</v>
       </c>
-      <c r="G25" s="27"/>
+      <c r="G25" s="40"/>
       <c r="H25" s="27"/>
       <c r="I25" s="27"/>
       <c r="J25" s="27"/>
@@ -9243,7 +9252,7 @@
       <c r="D26" s="23"/>
       <c r="E26" s="39"/>
       <c r="F26" s="39"/>
-      <c r="G26" s="23"/>
+      <c r="G26" s="39"/>
       <c r="H26" s="23" t="s">
         <v>64</v>
       </c>
@@ -9362,7 +9371,7 @@
       <c r="F33" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="27"/>
+      <c r="G33" s="40"/>
       <c r="H33" s="27"/>
       <c r="I33" s="27"/>
       <c r="J33" s="27" t="s">
@@ -9379,10 +9388,10 @@
       </c>
       <c r="E34" s="99"/>
       <c r="F34" s="99" t="s">
-        <v>537</v>
-      </c>
-      <c r="G34" s="98" t="s">
-        <v>521</v>
+        <v>536</v>
+      </c>
+      <c r="G34" s="99" t="s">
+        <v>520</v>
       </c>
       <c r="H34" s="98"/>
       <c r="I34" s="98"/>
@@ -9402,7 +9411,7 @@
       <c r="F35" s="40" t="s">
         <v>491</v>
       </c>
-      <c r="G35" s="27"/>
+      <c r="G35" s="40"/>
       <c r="H35" s="27"/>
       <c r="I35" s="27"/>
       <c r="J35" s="27" t="s">
@@ -9414,6 +9423,7 @@
       <c r="C36" s="23"/>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9541,7 +9551,7 @@
         <v>88</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F5" s="48" t="s">
         <v>90</v>
@@ -9635,10 +9645,10 @@
         <v>105</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F10" s="40" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H10" s="27" t="s">
         <v>103</v>
@@ -10858,7 +10868,7 @@
         <v>65</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F30" s="28" t="s">
         <v>190</v>
@@ -10938,7 +10948,7 @@
         <v>65</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F34" s="28" t="s">
         <v>190</v>
@@ -11090,7 +11100,7 @@
         <v>65</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F42" s="28" t="s">
         <v>190</v>
@@ -11170,10 +11180,10 @@
         <v>65</v>
       </c>
       <c r="E46" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="F46" s="28" t="s">
         <v>525</v>
-      </c>
-      <c r="F46" s="28" t="s">
-        <v>526</v>
       </c>
       <c r="G46" s="28"/>
       <c r="H46" s="26"/>
@@ -11250,10 +11260,10 @@
         <v>65</v>
       </c>
       <c r="E50" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="F50" s="28" t="s">
         <v>525</v>
-      </c>
-      <c r="F50" s="28" t="s">
-        <v>526</v>
       </c>
       <c r="G50" s="28"/>
       <c r="H50" s="26"/>
@@ -11330,10 +11340,10 @@
         <v>65</v>
       </c>
       <c r="E54" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="F54" s="28" t="s">
         <v>525</v>
-      </c>
-      <c r="F54" s="28" t="s">
-        <v>526</v>
       </c>
       <c r="G54" s="28"/>
       <c r="H54" s="26"/>
@@ -11442,7 +11452,7 @@
         <v>65</v>
       </c>
       <c r="E59" s="99" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F59" s="99" t="s">
         <v>449</v>
@@ -11485,7 +11495,7 @@
       </c>
       <c r="E61" s="99"/>
       <c r="F61" s="99" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G61" s="99"/>
       <c r="H61" s="98" t="s">
@@ -11507,7 +11517,7 @@
       </c>
       <c r="E62" s="105"/>
       <c r="F62" s="105" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G62" s="105"/>
       <c r="H62" s="104" t="s">
@@ -11890,7 +11900,7 @@
         <v>204</v>
       </c>
       <c r="F21" s="40" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G21" s="40" t="s">
         <v>494</v>
@@ -12691,7 +12701,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12821,12 +12831,15 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C7" s="27" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>242</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>542</v>
       </c>
       <c r="H7" s="27" t="s">
         <v>243</v>
@@ -12877,12 +12890,15 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="C11" s="27" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>250</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>541</v>
       </c>
       <c r="H11" s="27" t="s">
         <v>251</v>
@@ -13417,7 +13433,7 @@
         <v>222</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="H5" s="27" t="s">
         <v>224</v>
@@ -13434,7 +13450,7 @@
         <v>225</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="H6" s="27" t="s">
         <v>227</v>
@@ -13451,7 +13467,7 @@
         <v>228</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="H7" s="27" t="s">
         <v>230</v>
@@ -13468,10 +13484,10 @@
         <v>65</v>
       </c>
       <c r="E8" s="27" t="s">
+        <v>527</v>
+      </c>
+      <c r="F8" s="27" t="s">
         <v>528</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Saikļu tipi no tēzaura
</commit_message>
<xml_diff>
--- a/docs/SemTi-Kamols_morphotags.xlsx
+++ b/docs/SemTi-Kamols_morphotags.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20395"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pet/Documents/NLP/Treebank/Docs/Annotation how-to/Tags&amp;tagset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!LaumasDoc\Git\Treebank\Docs\Annotation how-to\Tags&amp;tagset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A50112-3477-0144-B3D7-C1C1F133486A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F51632-0BA4-47B4-8B7B-EE9AC85FF195}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="31500" windowHeight="20740" tabRatio="725" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="31500" windowHeight="20740" tabRatio="725" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par|About" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="799">
   <si>
     <t>Latviešu valodas morfoloģisko pazīmju kopa</t>
   </si>
@@ -5641,6 +5641,12 @@
   </si>
   <si>
     <t>nelokāms īpašības vārds, ja saskaņojas ar nelokāmu lietvārdu vai ģenitīveni</t>
+  </si>
+  <si>
+    <t>Sintaktiskā funkcija</t>
+  </si>
+  <si>
+    <t>Syntactic function</t>
   </si>
 </sst>
 </file>
@@ -6787,34 +6793,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="97.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="3.36328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="97.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B3" s="20" t="s">
         <v>726</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>722</v>
       </c>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>54</v>
       </c>
@@ -6822,7 +6828,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="8">
         <v>0</v>
       </c>
@@ -6830,13 +6836,13 @@
         <v>724</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>729</v>
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="21" t="s">
         <v>300</v>
       </c>
@@ -6844,7 +6850,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="10" t="s">
         <v>300</v>
       </c>
@@ -6862,29 +6868,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.36328125" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="12" max="12" width="23.36328125" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -6922,7 +6928,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -6954,15 +6960,15 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>2</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>18</v>
+        <v>797</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>391</v>
+        <v>798</v>
       </c>
       <c r="D3" s="54"/>
       <c r="E3" s="55"/>
@@ -6974,7 +6980,7 @@
       <c r="K3" s="54"/>
       <c r="L3" s="55"/>
     </row>
-    <row r="4" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D4" s="36" t="s">
         <v>3</v>
       </c>
@@ -6994,7 +7000,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="69"/>
       <c r="B5" s="70"/>
       <c r="C5" s="71"/>
@@ -7020,7 +7026,7 @@
       </c>
       <c r="L5" s="70"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="53"/>
       <c r="B6" s="55"/>
       <c r="C6" s="61"/>
@@ -7049,24 +7055,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.453125" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="12" max="12" width="23.36328125" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -7104,7 +7110,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -7138,7 +7144,7 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="53"/>
       <c r="B3" s="55"/>
       <c r="C3" s="61"/>
@@ -7166,24 +7172,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6328125" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="12" max="12" width="23.36328125" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -7221,7 +7227,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -7255,7 +7261,7 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="53"/>
       <c r="B3" s="55"/>
       <c r="C3" s="61"/>
@@ -7283,24 +7289,24 @@
       <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.1640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="67.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.36328125" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" style="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.36328125" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="67.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -7338,7 +7344,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -7372,7 +7378,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>2</v>
       </c>
@@ -7392,7 +7398,7 @@
       <c r="K3" s="54"/>
       <c r="L3" s="55"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B4" s="41"/>
       <c r="C4" s="42"/>
       <c r="D4" s="36" t="s">
@@ -7414,7 +7420,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D5" s="36" t="s">
         <v>174</v>
       </c>
@@ -7437,7 +7443,7 @@
         <v>2081</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
@@ -7463,7 +7469,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>286</v>
       </c>
@@ -7489,7 +7495,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D8" s="36" t="s">
         <v>34</v>
       </c>
@@ -7512,7 +7518,7 @@
         <v>2077</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D9" s="36" t="s">
         <v>68</v>
       </c>
@@ -7532,7 +7538,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="69"/>
       <c r="B10" s="70"/>
       <c r="C10" s="71"/>
@@ -7556,7 +7562,7 @@
       <c r="K10" s="72"/>
       <c r="L10" s="70"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="53"/>
       <c r="B11" s="55"/>
       <c r="C11" s="61"/>
@@ -7585,24 +7591,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.1640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="12" max="12" width="23.36328125" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -7640,7 +7646,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -7676,7 +7682,7 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>2</v>
       </c>
@@ -7706,7 +7712,7 @@
       <c r="K3" s="133"/>
       <c r="L3" s="134"/>
     </row>
-    <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="35"/>
       <c r="B4" s="37"/>
       <c r="C4" s="43"/>
@@ -7730,7 +7736,7 @@
       <c r="K4" s="126"/>
       <c r="L4" s="127"/>
     </row>
-    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="35"/>
       <c r="B5" s="37"/>
       <c r="C5" s="43"/>
@@ -7752,7 +7758,7 @@
       <c r="K5" s="126"/>
       <c r="L5" s="127"/>
     </row>
-    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="35"/>
       <c r="B6" s="37"/>
       <c r="C6" s="43"/>
@@ -7774,7 +7780,7 @@
       <c r="K6" s="126"/>
       <c r="L6" s="127"/>
     </row>
-    <row r="7" spans="1:12" s="125" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="125" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="128"/>
       <c r="B7" s="129"/>
       <c r="C7" s="130"/>
@@ -7796,7 +7802,7 @@
       <c r="K7" s="131"/>
       <c r="L7" s="129"/>
     </row>
-    <row r="8" spans="1:12" s="125" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="125" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="135"/>
       <c r="B8" s="136"/>
       <c r="C8" s="137"/>
@@ -7818,7 +7824,7 @@
       <c r="K8" s="138"/>
       <c r="L8" s="136"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="53"/>
       <c r="B9" s="55"/>
       <c r="C9" s="61"/>
@@ -7847,24 +7853,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.81640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.453125" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.453125" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.6328125" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1796875" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="12" max="12" width="23.36328125" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -7902,7 +7908,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -7936,7 +7942,7 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>2</v>
       </c>
@@ -7966,7 +7972,7 @@
       <c r="K3" s="54"/>
       <c r="L3" s="55"/>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D4" s="36" t="s">
         <v>68</v>
       </c>
@@ -7983,7 +7989,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D5" s="36" t="s">
         <v>9</v>
       </c>
@@ -8000,7 +8006,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>135</v>
       </c>
@@ -8018,7 +8024,7 @@
       </c>
       <c r="I6" s="110"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="69"/>
       <c r="B7" s="70"/>
       <c r="C7" s="71"/>
@@ -8040,7 +8046,7 @@
       <c r="K7" s="72"/>
       <c r="L7" s="70"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="53"/>
       <c r="B8" s="55"/>
       <c r="C8" s="61"/>
@@ -8067,25 +8073,25 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" style="18" customWidth="1"/>
     <col min="2" max="2" width="2" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="49" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" style="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="49" customWidth="1"/>
-    <col min="7" max="7" width="14.5" style="50" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" style="49" customWidth="1"/>
+    <col min="3" max="3" width="24.6328125" style="49" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" style="52" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.6328125" style="49" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" style="50" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6328125" style="49" customWidth="1"/>
     <col min="9" max="9" width="21" style="52" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" style="49" customWidth="1"/>
-    <col min="11" max="11" width="15.5" style="52" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.6328125" style="49" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" style="52" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="52" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="53" style="49" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="18"/>
+    <col min="14" max="16384" width="8.81640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>732</v>
       </c>
@@ -8102,7 +8108,7 @@
       <c r="L1" s="18"/>
       <c r="M1" s="18"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8121,7 +8127,7 @@
       <c r="L2" s="18"/>
       <c r="M2" s="18"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8140,13 +8146,13 @@
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>725</v>
       </c>
       <c r="B4" s="157"/>
     </row>
-    <row r="5" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A5" s="142" t="s">
         <v>764</v>
       </c>
@@ -8163,22 +8169,22 @@
       <c r="L5" s="18"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>765</v>
       </c>
       <c r="B6" s="157"/>
     </row>
-    <row r="7" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>782</v>
       </c>
       <c r="B7" s="157"/>
     </row>
-    <row r="8" spans="1:14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="157"/>
     </row>
-    <row r="9" spans="1:14" ht="19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A9" s="142" t="s">
         <v>670</v>
       </c>
@@ -8195,7 +8201,7 @@
       <c r="L9" s="18"/>
       <c r="M9" s="18"/>
     </row>
-    <row r="10" spans="1:14" s="143" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="143" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="145" t="s">
         <v>406</v>
       </c>
@@ -8236,7 +8242,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>405</v>
       </c>
@@ -8275,7 +8281,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12" s="53">
         <v>5</v>
       </c>
@@ -8307,7 +8313,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="69"/>
       <c r="C13" s="102"/>
       <c r="D13" s="103"/>
@@ -8321,7 +8327,7 @@
       <c r="L13" s="107"/>
       <c r="M13" s="102"/>
     </row>
-    <row r="14" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>454</v>
       </c>
@@ -8354,7 +8360,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="69"/>
       <c r="C15" s="102"/>
       <c r="D15" s="103"/>
@@ -8368,7 +8374,7 @@
       <c r="L15" s="107"/>
       <c r="M15" s="102"/>
     </row>
-    <row r="16" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>519</v>
       </c>
@@ -8402,7 +8408,7 @@
       </c>
       <c r="N16" s="9"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B17" s="69"/>
       <c r="C17" s="102"/>
       <c r="D17" s="103"/>
@@ -8416,7 +8422,7 @@
       <c r="L17" s="107"/>
       <c r="M17" s="102"/>
     </row>
-    <row r="18" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>554</v>
       </c>
@@ -8449,7 +8455,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C19" s="37"/>
       <c r="D19" s="43"/>
       <c r="E19" s="36" t="s">
@@ -8470,7 +8476,7 @@
       <c r="L19" s="36"/>
       <c r="M19" s="37"/>
     </row>
-    <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="C20" s="37"/>
       <c r="D20" s="43"/>
       <c r="E20" s="36" t="s">
@@ -8491,7 +8497,7 @@
       <c r="L20" s="36"/>
       <c r="M20" s="37"/>
     </row>
-    <row r="21" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="C21" s="37"/>
       <c r="D21" s="43"/>
       <c r="E21" s="36" t="s">
@@ -8512,7 +8518,7 @@
       <c r="L21" s="36"/>
       <c r="M21" s="37"/>
     </row>
-    <row r="22" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="C22" s="37"/>
       <c r="D22" s="43"/>
       <c r="E22" s="36" t="s">
@@ -8533,7 +8539,7 @@
       <c r="L22" s="36"/>
       <c r="M22" s="37"/>
     </row>
-    <row r="23" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C23" s="37"/>
       <c r="D23" s="43"/>
       <c r="E23" s="36" t="s">
@@ -8552,7 +8558,7 @@
       <c r="L23" s="36"/>
       <c r="M23" s="37"/>
     </row>
-    <row r="24" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C24" s="37"/>
       <c r="D24" s="43"/>
       <c r="E24" s="36" t="s">
@@ -8571,7 +8577,7 @@
       <c r="L24" s="36"/>
       <c r="M24" s="37"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B25" s="69"/>
       <c r="C25" s="102"/>
       <c r="D25" s="103"/>
@@ -8585,7 +8591,7 @@
       <c r="L25" s="107"/>
       <c r="M25" s="102"/>
     </row>
-    <row r="26" spans="1:13" s="144" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="144" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>564</v>
       </c>
@@ -8614,7 +8620,7 @@
       <c r="L26" s="151"/>
       <c r="M26" s="156"/>
     </row>
-    <row r="27" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="C27" s="37"/>
       <c r="D27" s="43"/>
       <c r="E27" s="36" t="s">
@@ -8633,7 +8639,7 @@
       <c r="K27" s="36"/>
       <c r="L27" s="36"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C28" s="37"/>
       <c r="D28" s="43"/>
       <c r="E28" s="36">
@@ -8649,7 +8655,7 @@
       <c r="K28" s="36"/>
       <c r="L28" s="36"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B29" s="69"/>
       <c r="C29" s="102"/>
       <c r="D29" s="103"/>
@@ -8663,7 +8669,7 @@
       <c r="L29" s="107"/>
       <c r="M29" s="102"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
         <v>598</v>
       </c>
@@ -8684,7 +8690,7 @@
       <c r="L30" s="82"/>
       <c r="M30" s="78"/>
     </row>
-    <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C31" s="37"/>
       <c r="E31" s="36" t="s">
         <v>59</v>
@@ -8701,7 +8707,7 @@
       <c r="J31" s="37"/>
       <c r="K31" s="36"/>
     </row>
-    <row r="32" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C32" s="37"/>
       <c r="E32" s="36" t="s">
         <v>9</v>
@@ -8718,7 +8724,7 @@
       <c r="J32" s="37"/>
       <c r="K32" s="36"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B33" s="69"/>
       <c r="C33" s="102"/>
       <c r="D33" s="103"/>
@@ -8732,7 +8738,7 @@
       <c r="L33" s="107"/>
       <c r="M33" s="102"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>611</v>
       </c>
@@ -8757,7 +8763,7 @@
       <c r="L34" s="54"/>
       <c r="M34" s="55"/>
     </row>
-    <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C35" s="41"/>
       <c r="D35" s="42"/>
       <c r="E35" s="36" t="s">
@@ -8780,7 +8786,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C36" s="37"/>
       <c r="D36" s="43"/>
       <c r="E36" s="36" t="s">
@@ -8801,7 +8807,7 @@
       <c r="L36" s="36"/>
       <c r="M36" s="37"/>
     </row>
-    <row r="37" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C37" s="37"/>
       <c r="D37" s="43"/>
       <c r="E37" s="36" t="s">
@@ -8824,7 +8830,7 @@
       <c r="L37" s="36"/>
       <c r="M37" s="37"/>
     </row>
-    <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C38" s="37"/>
       <c r="D38" s="43"/>
       <c r="E38" s="36" t="s">
@@ -8845,7 +8851,7 @@
       <c r="L38" s="36"/>
       <c r="M38" s="37"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B39" s="69"/>
       <c r="C39" s="70"/>
       <c r="D39" s="71"/>
@@ -8859,7 +8865,7 @@
       <c r="L39" s="72"/>
       <c r="M39" s="70"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="14" t="s">
         <v>620</v>
       </c>
@@ -8884,7 +8890,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C41" s="41"/>
       <c r="D41" s="42"/>
       <c r="E41" s="36" t="s">
@@ -8904,7 +8910,7 @@
       <c r="K41" s="36"/>
       <c r="L41" s="36"/>
     </row>
-    <row r="42" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="C42" s="37"/>
       <c r="D42" s="43"/>
       <c r="E42" s="36" t="s">
@@ -8925,7 +8931,7 @@
       <c r="L42" s="36"/>
       <c r="M42" s="37"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B43" s="69"/>
       <c r="C43" s="102"/>
       <c r="D43" s="103"/>
@@ -8939,7 +8945,7 @@
       <c r="L43" s="107"/>
       <c r="M43" s="102"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="14" t="s">
         <v>634</v>
       </c>
@@ -8964,7 +8970,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C45" s="41"/>
       <c r="D45" s="42"/>
       <c r="E45" s="36" t="s">
@@ -8983,7 +8989,7 @@
       <c r="J45" s="37"/>
       <c r="K45" s="36"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C46" s="37"/>
       <c r="D46" s="43"/>
       <c r="E46" s="36" t="s">
@@ -9003,7 +9009,7 @@
       <c r="K46" s="36"/>
       <c r="L46" s="36"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B47" s="69"/>
       <c r="C47" s="102"/>
       <c r="D47" s="103"/>
@@ -9017,7 +9023,7 @@
       <c r="L47" s="107"/>
       <c r="M47" s="102"/>
     </row>
-    <row r="48" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="14" t="s">
         <v>669</v>
       </c>
@@ -9048,7 +9054,7 @@
       <c r="L48" s="160"/>
       <c r="M48" s="161"/>
     </row>
-    <row r="49" spans="2:13" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B49" s="53"/>
       <c r="C49" s="78"/>
       <c r="D49" s="79"/>
@@ -9077,24 +9083,24 @@
       <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="49" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="50" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" style="48" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.1640625" style="51" customWidth="1"/>
-    <col min="9" max="9" width="33.6640625" style="48" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="52" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.36328125" style="48" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1796875" style="51" customWidth="1"/>
+    <col min="9" max="9" width="33.6328125" style="48" customWidth="1"/>
+    <col min="10" max="10" width="19.36328125" style="52" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="52" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5" style="49" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="18"/>
+    <col min="12" max="12" width="23.453125" style="49" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="62" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="62" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -9132,7 +9138,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -9162,7 +9168,7 @@
       <c r="K2" s="28"/>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>2</v>
       </c>
@@ -9182,7 +9188,7 @@
       <c r="K3" s="54"/>
       <c r="L3" s="55"/>
     </row>
-    <row r="4" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B4" s="37"/>
       <c r="C4" s="43"/>
       <c r="D4" s="36" t="s">
@@ -9211,7 +9217,7 @@
       </c>
       <c r="L4" s="37"/>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="69"/>
       <c r="B5" s="70"/>
       <c r="C5" s="71"/>
@@ -9239,7 +9245,7 @@
       </c>
       <c r="L5" s="70"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="53">
         <v>3</v>
       </c>
@@ -9263,7 +9269,7 @@
       </c>
       <c r="L6" s="55"/>
     </row>
-    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="37"/>
       <c r="C7" s="43"/>
       <c r="D7" s="36" t="s">
@@ -9290,7 +9296,7 @@
       </c>
       <c r="L7" s="37"/>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" s="37"/>
       <c r="C8" s="43"/>
       <c r="D8" s="36" t="s">
@@ -9315,7 +9321,7 @@
       </c>
       <c r="L8" s="37"/>
     </row>
-    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="69"/>
       <c r="B9" s="70"/>
       <c r="C9" s="71"/>
@@ -9339,7 +9345,7 @@
       <c r="K9" s="72"/>
       <c r="L9" s="70"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="53">
         <v>4</v>
       </c>
@@ -9363,7 +9369,7 @@
       </c>
       <c r="L10" s="55"/>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" s="37"/>
       <c r="C11" s="43"/>
       <c r="D11" s="36" t="s">
@@ -9388,7 +9394,7 @@
       </c>
       <c r="L11" s="37"/>
     </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B12" s="37"/>
       <c r="C12" s="43"/>
       <c r="D12" s="36" t="s">
@@ -9413,7 +9419,7 @@
       </c>
       <c r="L12" s="37"/>
     </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B13" s="37"/>
       <c r="C13" s="43"/>
       <c r="D13" s="36" t="s">
@@ -9438,7 +9444,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="37"/>
       <c r="C14" s="43"/>
       <c r="D14" s="36" t="s">
@@ -9465,7 +9471,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="69"/>
       <c r="B15" s="70"/>
       <c r="C15" s="71"/>
@@ -9487,7 +9493,7 @@
       <c r="K15" s="72"/>
       <c r="L15" s="70"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="53">
         <v>5</v>
       </c>
@@ -9511,7 +9517,7 @@
       </c>
       <c r="L16" s="55"/>
     </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B17" s="37"/>
       <c r="C17" s="43"/>
       <c r="D17" s="36" t="s">
@@ -9536,7 +9542,7 @@
       </c>
       <c r="L17" s="37"/>
     </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B18" s="37"/>
       <c r="C18" s="43"/>
       <c r="D18" s="36" t="s">
@@ -9561,7 +9567,7 @@
       </c>
       <c r="L18" s="37"/>
     </row>
-    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B19" s="37"/>
       <c r="C19" s="43"/>
       <c r="D19" s="36" t="s">
@@ -9586,7 +9592,7 @@
       </c>
       <c r="L19" s="37"/>
     </row>
-    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B20" s="37"/>
       <c r="C20" s="43"/>
       <c r="D20" s="36" t="s">
@@ -9611,7 +9617,7 @@
       </c>
       <c r="L20" s="37"/>
     </row>
-    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B21" s="37"/>
       <c r="C21" s="43"/>
       <c r="D21" s="36" t="s">
@@ -9636,7 +9642,7 @@
       </c>
       <c r="L21" s="37"/>
     </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B22" s="37"/>
       <c r="C22" s="43"/>
       <c r="D22" s="36" t="s">
@@ -9661,7 +9667,7 @@
       </c>
       <c r="L22" s="37"/>
     </row>
-    <row r="23" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="69"/>
       <c r="B23" s="70"/>
       <c r="C23" s="71"/>
@@ -9685,7 +9691,7 @@
       <c r="K23" s="72"/>
       <c r="L23" s="70"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="53">
         <v>6</v>
       </c>
@@ -9709,7 +9715,7 @@
       </c>
       <c r="L24" s="55"/>
     </row>
-    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B25" s="37"/>
       <c r="C25" s="43"/>
       <c r="D25" s="36">
@@ -9729,7 +9735,7 @@
       <c r="K25" s="36"/>
       <c r="L25" s="37"/>
     </row>
-    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B26" s="37"/>
       <c r="C26" s="43"/>
       <c r="D26" s="36">
@@ -9749,7 +9755,7 @@
       <c r="K26" s="36"/>
       <c r="L26" s="37"/>
     </row>
-    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B27" s="37"/>
       <c r="C27" s="43"/>
       <c r="D27" s="36">
@@ -9769,7 +9775,7 @@
       <c r="K27" s="36"/>
       <c r="L27" s="37"/>
     </row>
-    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B28" s="37"/>
       <c r="C28" s="43"/>
       <c r="D28" s="36">
@@ -9789,7 +9795,7 @@
       <c r="K28" s="36"/>
       <c r="L28" s="37"/>
     </row>
-    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B29" s="37"/>
       <c r="C29" s="43"/>
       <c r="D29" s="36">
@@ -9809,7 +9815,7 @@
       <c r="K29" s="36"/>
       <c r="L29" s="37"/>
     </row>
-    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B30" s="37"/>
       <c r="C30" s="43"/>
       <c r="D30" s="36">
@@ -9829,7 +9835,7 @@
       <c r="K30" s="36"/>
       <c r="L30" s="37"/>
     </row>
-    <row r="31" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B31" s="37"/>
       <c r="C31" s="43"/>
       <c r="D31" s="36">
@@ -9854,7 +9860,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B32" s="37"/>
       <c r="C32" s="43"/>
       <c r="D32" s="36" t="s">
@@ -9879,7 +9885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="69"/>
       <c r="B33" s="70"/>
       <c r="C33" s="71"/>
@@ -9903,7 +9909,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="53"/>
       <c r="B34" s="78"/>
       <c r="C34" s="79"/>
@@ -9932,24 +9938,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="99" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" style="39" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.81640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.6328125" style="39" customWidth="1"/>
+    <col min="8" max="8" width="30.6328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.453125" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.36328125" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="52.5" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="12" max="12" width="52.453125" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -9987,7 +9993,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="30">
         <v>1</v>
       </c>
@@ -10019,7 +10025,7 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="109">
         <v>2</v>
       </c>
@@ -10041,7 +10047,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D4" s="36" t="s">
         <v>5</v>
       </c>
@@ -10061,7 +10067,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D5" s="36" t="s">
         <v>68</v>
       </c>
@@ -10084,7 +10090,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>4</v>
       </c>
@@ -10104,7 +10110,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>73</v>
       </c>
@@ -10124,7 +10130,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D8" s="36" t="s">
         <v>3</v>
       </c>
@@ -10147,7 +10153,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="158"/>
       <c r="B9" s="70"/>
       <c r="C9" s="71"/>
@@ -10177,7 +10183,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="158"/>
       <c r="B10" s="70"/>
       <c r="C10" s="71"/>
@@ -10207,7 +10213,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="109">
         <v>3</v>
       </c>
@@ -10229,7 +10235,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D12" s="36" t="s">
         <v>9</v>
       </c>
@@ -10249,7 +10255,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D13" s="36" t="s">
         <v>59</v>
       </c>
@@ -10269,7 +10275,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="158"/>
       <c r="B14" s="70"/>
       <c r="C14" s="71"/>
@@ -10291,7 +10297,7 @@
       <c r="K14" s="89"/>
       <c r="L14" s="90"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="109">
         <v>4</v>
       </c>
@@ -10317,7 +10323,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D16" s="36" t="s">
         <v>87</v>
       </c>
@@ -10337,7 +10343,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D17" s="36" t="s">
         <v>14</v>
       </c>
@@ -10354,7 +10360,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D18" s="36" t="s">
         <v>3</v>
       </c>
@@ -10374,7 +10380,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D19" s="36" t="s">
         <v>34</v>
       </c>
@@ -10394,7 +10400,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D20" s="36" t="s">
         <v>5</v>
       </c>
@@ -10414,7 +10420,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D21" s="36" t="s">
         <v>9</v>
       </c>
@@ -10434,7 +10440,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B22" s="70"/>
       <c r="C22" s="71"/>
       <c r="D22" s="72" t="s">
@@ -10461,7 +10467,7 @@
       </c>
       <c r="L22" s="70"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="99">
         <v>5</v>
       </c>
@@ -10485,7 +10491,7 @@
       </c>
       <c r="L23" s="55"/>
     </row>
-    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D24" s="36" t="s">
         <v>4</v>
       </c>
@@ -10505,7 +10511,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D25" s="36" t="s">
         <v>6</v>
       </c>
@@ -10525,7 +10531,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D26" s="36" t="s">
         <v>8</v>
       </c>
@@ -10545,7 +10551,7 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="158"/>
       <c r="B27" s="70"/>
       <c r="C27" s="71"/>
@@ -10569,7 +10575,7 @@
       <c r="K27" s="72"/>
       <c r="L27" s="70"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="109">
         <v>6</v>
       </c>
@@ -10589,7 +10595,7 @@
       <c r="K28" s="54"/>
       <c r="L28" s="55"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D29" s="36" t="s">
         <v>78</v>
       </c>
@@ -10606,7 +10612,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D30" s="36" t="s">
         <v>87</v>
       </c>
@@ -10623,7 +10629,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="158"/>
       <c r="B31" s="70"/>
       <c r="C31" s="71"/>
@@ -10645,7 +10651,7 @@
       <c r="K31" s="72"/>
       <c r="L31" s="70"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="109">
         <v>7</v>
       </c>
@@ -10669,7 +10675,7 @@
       </c>
       <c r="L32" s="55"/>
     </row>
-    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D33" s="36">
         <v>1</v>
       </c>
@@ -10683,7 +10689,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D34" s="36">
         <v>2</v>
       </c>
@@ -10697,7 +10703,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D35" s="36">
         <v>3</v>
       </c>
@@ -10711,7 +10717,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D36" s="36" t="s">
         <v>87</v>
       </c>
@@ -10728,7 +10734,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="158"/>
       <c r="B37" s="70"/>
       <c r="C37" s="71"/>
@@ -10750,7 +10756,7 @@
       <c r="K37" s="72"/>
       <c r="L37" s="70"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="109">
         <v>8</v>
       </c>
@@ -10774,7 +10780,7 @@
       </c>
       <c r="L38" s="55"/>
     </row>
-    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D39" s="36">
         <v>1</v>
       </c>
@@ -10788,7 +10794,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D40" s="36">
         <v>2</v>
       </c>
@@ -10802,7 +10808,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D41" s="36">
         <v>3</v>
       </c>
@@ -10816,7 +10822,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="158"/>
       <c r="B42" s="70"/>
       <c r="C42" s="71"/>
@@ -10838,7 +10844,7 @@
       <c r="K42" s="72"/>
       <c r="L42" s="70"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="109">
         <v>9</v>
       </c>
@@ -10862,7 +10868,7 @@
       </c>
       <c r="L43" s="55"/>
     </row>
-    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D44" s="36" t="s">
         <v>8</v>
       </c>
@@ -10882,7 +10888,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D45" s="36" t="s">
         <v>4</v>
       </c>
@@ -10902,7 +10908,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A46" s="158"/>
       <c r="B46" s="70"/>
       <c r="C46" s="71"/>
@@ -10926,7 +10932,7 @@
       <c r="K46" s="72"/>
       <c r="L46" s="70"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="109">
         <v>10</v>
       </c>
@@ -10950,7 +10956,7 @@
       </c>
       <c r="L47" s="55"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D48" s="36" t="s">
         <v>11</v>
       </c>
@@ -10967,7 +10973,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D49" s="36" t="s">
         <v>4</v>
       </c>
@@ -10987,7 +10993,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="158"/>
       <c r="B50" s="70"/>
       <c r="C50" s="71"/>
@@ -11009,7 +11015,7 @@
       <c r="K50" s="72"/>
       <c r="L50" s="70"/>
     </row>
-    <row r="51" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="109">
         <v>11</v>
       </c>
@@ -11037,7 +11043,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D52" s="36" t="s">
         <v>9</v>
       </c>
@@ -11057,7 +11063,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="158"/>
       <c r="B53" s="70"/>
       <c r="C53" s="71"/>
@@ -11083,7 +11089,7 @@
       </c>
       <c r="L53" s="70"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="109"/>
       <c r="B54" s="55"/>
       <c r="C54" s="61"/>
@@ -11112,24 +11118,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5" style="39" customWidth="1"/>
-    <col min="8" max="8" width="28.5" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.5" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6328125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.453125" style="39" customWidth="1"/>
+    <col min="8" max="8" width="28.453125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.453125" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.36328125" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="52.5" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="12" max="12" width="52.453125" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -11167,7 +11173,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -11199,7 +11205,7 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>2</v>
       </c>
@@ -11221,7 +11227,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D4" s="36" t="s">
         <v>5</v>
       </c>
@@ -11241,7 +11247,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D5" s="36" t="s">
         <v>68</v>
       </c>
@@ -11264,7 +11270,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>4</v>
       </c>
@@ -11284,7 +11290,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>73</v>
       </c>
@@ -11304,7 +11310,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D8" s="36" t="s">
         <v>3</v>
       </c>
@@ -11327,7 +11333,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="69"/>
       <c r="B9" s="70"/>
       <c r="C9" s="71"/>
@@ -11357,7 +11363,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="69"/>
       <c r="B10" s="70"/>
       <c r="C10" s="71"/>
@@ -11387,7 +11393,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="53">
         <v>3</v>
       </c>
@@ -11409,7 +11415,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D12" s="36" t="s">
         <v>9</v>
       </c>
@@ -11429,7 +11435,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D13" s="36" t="s">
         <v>59</v>
       </c>
@@ -11449,7 +11455,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="69"/>
       <c r="B14" s="70"/>
       <c r="C14" s="71"/>
@@ -11471,7 +11477,7 @@
       <c r="K14" s="89"/>
       <c r="L14" s="90"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="53">
         <v>4</v>
       </c>
@@ -11497,7 +11503,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D16" s="36" t="s">
         <v>87</v>
       </c>
@@ -11520,7 +11526,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D17" s="36" t="s">
         <v>14</v>
       </c>
@@ -11540,7 +11546,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D18" s="36" t="s">
         <v>3</v>
       </c>
@@ -11563,7 +11569,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D19" s="36" t="s">
         <v>34</v>
       </c>
@@ -11583,7 +11589,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D20" s="36" t="s">
         <v>5</v>
       </c>
@@ -11606,7 +11612,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D21" s="36" t="s">
         <v>9</v>
       </c>
@@ -11629,7 +11635,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="69"/>
       <c r="B22" s="70"/>
       <c r="C22" s="71"/>
@@ -11655,7 +11661,7 @@
       </c>
       <c r="L22" s="70"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="53">
         <v>5</v>
       </c>
@@ -11679,7 +11685,7 @@
       </c>
       <c r="L23" s="78"/>
     </row>
-    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B24" s="49"/>
       <c r="C24" s="50"/>
       <c r="D24" s="36" t="s">
@@ -11704,7 +11710,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B25" s="49"/>
       <c r="C25" s="50"/>
       <c r="D25" s="36" t="s">
@@ -11729,7 +11735,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="69"/>
       <c r="B26" s="102"/>
       <c r="C26" s="103"/>
@@ -11755,7 +11761,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="53">
         <v>6</v>
       </c>
@@ -11779,7 +11785,7 @@
       </c>
       <c r="L27" s="78"/>
     </row>
-    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B28" s="49"/>
       <c r="C28" s="50"/>
       <c r="D28" s="36" t="s">
@@ -11804,7 +11810,7 @@
       </c>
       <c r="L28" s="49"/>
     </row>
-    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B29" s="49"/>
       <c r="C29" s="50"/>
       <c r="D29" s="36" t="s">
@@ -11829,7 +11835,7 @@
       </c>
       <c r="L29" s="49"/>
     </row>
-    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="69"/>
       <c r="B30" s="102"/>
       <c r="C30" s="103"/>
@@ -11853,7 +11859,7 @@
       <c r="K30" s="107"/>
       <c r="L30" s="102"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="53">
         <v>7</v>
       </c>
@@ -11877,7 +11883,7 @@
       </c>
       <c r="L31" s="78"/>
     </row>
-    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B32" s="49"/>
       <c r="C32" s="50"/>
       <c r="D32" s="36" t="s">
@@ -11902,7 +11908,7 @@
       </c>
       <c r="L32" s="49"/>
     </row>
-    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B33" s="49"/>
       <c r="C33" s="50"/>
       <c r="D33" s="36" t="s">
@@ -11927,7 +11933,7 @@
       </c>
       <c r="L33" s="49"/>
     </row>
-    <row r="34" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="69"/>
       <c r="B34" s="102"/>
       <c r="C34" s="103"/>
@@ -11951,7 +11957,7 @@
       <c r="K34" s="107"/>
       <c r="L34" s="102"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="53">
         <v>8</v>
       </c>
@@ -11975,7 +11981,7 @@
       </c>
       <c r="L35" s="78"/>
     </row>
-    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B36" s="49"/>
       <c r="C36" s="50"/>
       <c r="D36" s="36" t="s">
@@ -12000,7 +12006,7 @@
       </c>
       <c r="L36" s="49"/>
     </row>
-    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B37" s="49"/>
       <c r="C37" s="50"/>
       <c r="D37" s="36" t="s">
@@ -12025,7 +12031,7 @@
       </c>
       <c r="L37" s="49"/>
     </row>
-    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B38" s="49"/>
       <c r="C38" s="50"/>
       <c r="D38" s="36" t="s">
@@ -12050,7 +12056,7 @@
       </c>
       <c r="L38" s="49"/>
     </row>
-    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B39" s="49"/>
       <c r="C39" s="50"/>
       <c r="D39" s="36" t="s">
@@ -12075,7 +12081,7 @@
       </c>
       <c r="L39" s="49"/>
     </row>
-    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B40" s="49"/>
       <c r="C40" s="50"/>
       <c r="D40" s="36" t="s">
@@ -12100,7 +12106,7 @@
       </c>
       <c r="L40" s="49"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B41" s="49"/>
       <c r="C41" s="50"/>
       <c r="D41" s="36" t="s">
@@ -12123,7 +12129,7 @@
       </c>
       <c r="L41" s="49"/>
     </row>
-    <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="69"/>
       <c r="B42" s="102"/>
       <c r="C42" s="103"/>
@@ -12147,7 +12153,7 @@
       <c r="K42" s="107"/>
       <c r="L42" s="102"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="53">
         <v>9</v>
       </c>
@@ -12171,7 +12177,7 @@
       </c>
       <c r="L43" s="78"/>
     </row>
-    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B44" s="49"/>
       <c r="C44" s="50"/>
       <c r="D44" s="36" t="s">
@@ -12198,7 +12204,7 @@
       </c>
       <c r="L44" s="49"/>
     </row>
-    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B45" s="49"/>
       <c r="C45" s="50"/>
       <c r="D45" s="36" t="s">
@@ -12225,7 +12231,7 @@
       </c>
       <c r="L45" s="49"/>
     </row>
-    <row r="46" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="69"/>
       <c r="B46" s="102"/>
       <c r="C46" s="103"/>
@@ -12249,7 +12255,7 @@
       <c r="K46" s="107"/>
       <c r="L46" s="102"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="53">
         <v>10</v>
       </c>
@@ -12273,7 +12279,7 @@
       </c>
       <c r="L47" s="78"/>
     </row>
-    <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B48" s="49"/>
       <c r="C48" s="50"/>
       <c r="D48" s="36" t="s">
@@ -12300,7 +12306,7 @@
       </c>
       <c r="L48" s="49"/>
     </row>
-    <row r="49" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B49" s="49"/>
       <c r="C49" s="50"/>
       <c r="D49" s="36" t="s">
@@ -12327,7 +12333,7 @@
       </c>
       <c r="L49" s="49"/>
     </row>
-    <row r="50" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="69"/>
       <c r="B50" s="102"/>
       <c r="C50" s="103"/>
@@ -12351,7 +12357,7 @@
       <c r="K50" s="107"/>
       <c r="L50" s="102"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="53">
         <v>11</v>
       </c>
@@ -12375,7 +12381,7 @@
       </c>
       <c r="L51" s="78"/>
     </row>
-    <row r="52" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B52" s="49"/>
       <c r="C52" s="50"/>
       <c r="D52" s="36" t="s">
@@ -12400,7 +12406,7 @@
       </c>
       <c r="L52" s="49"/>
     </row>
-    <row r="53" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B53" s="49"/>
       <c r="C53" s="50"/>
       <c r="D53" s="36" t="s">
@@ -12425,7 +12431,7 @@
       </c>
       <c r="L53" s="49"/>
     </row>
-    <row r="54" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="69"/>
       <c r="B54" s="102"/>
       <c r="C54" s="103"/>
@@ -12449,7 +12455,7 @@
       <c r="K54" s="107"/>
       <c r="L54" s="49"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="53">
         <v>12</v>
       </c>
@@ -12472,7 +12478,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D56" s="36" t="s">
         <v>4</v>
       </c>
@@ -12495,7 +12501,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D57" s="36" t="s">
         <v>3</v>
       </c>
@@ -12518,7 +12524,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D58" s="36" t="s">
         <v>8</v>
       </c>
@@ -12541,7 +12547,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="69"/>
       <c r="B59" s="70"/>
       <c r="C59" s="71"/>
@@ -12565,7 +12571,7 @@
       <c r="K59" s="72"/>
       <c r="L59" s="70"/>
     </row>
-    <row r="60" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A60" s="109">
         <v>13</v>
       </c>
@@ -12593,7 +12599,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="84"/>
       <c r="D61" s="36" t="s">
         <v>9</v>
@@ -12614,7 +12620,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="88"/>
       <c r="B62" s="70"/>
       <c r="C62" s="71"/>
@@ -12640,7 +12646,7 @@
       </c>
       <c r="L62" s="70"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="53"/>
       <c r="B63" s="55"/>
       <c r="C63" s="61"/>
@@ -12664,29 +12670,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5" style="39" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.33203125" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.453125" style="39" customWidth="1"/>
+    <col min="8" max="8" width="23.36328125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.36328125" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.36328125" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="12" max="12" width="23.36328125" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -12724,7 +12730,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -12756,7 +12762,7 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>2</v>
       </c>
@@ -12776,7 +12782,7 @@
       <c r="K3" s="54"/>
       <c r="L3" s="55"/>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D4" s="36" t="s">
         <v>6</v>
       </c>
@@ -12796,7 +12802,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="69"/>
       <c r="B5" s="70"/>
       <c r="C5" s="71"/>
@@ -12820,7 +12826,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="53">
         <v>3</v>
       </c>
@@ -12848,7 +12854,7 @@
       </c>
       <c r="L6" s="55"/>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>5</v>
       </c>
@@ -12868,7 +12874,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="69"/>
       <c r="B8" s="70"/>
       <c r="C8" s="71"/>
@@ -12894,7 +12900,7 @@
       </c>
       <c r="L8" s="70"/>
     </row>
-    <row r="9" spans="1:12" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="18" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="69"/>
       <c r="B9" s="70"/>
       <c r="C9" s="71"/>
@@ -12918,7 +12924,7 @@
       <c r="K9" s="72"/>
       <c r="L9" s="70"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="53">
         <v>4</v>
       </c>
@@ -12942,7 +12948,7 @@
       </c>
       <c r="L10" s="55"/>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D11" s="36" t="s">
         <v>8</v>
       </c>
@@ -12962,7 +12968,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="69"/>
       <c r="B12" s="70"/>
       <c r="C12" s="71"/>
@@ -12988,7 +12994,7 @@
       </c>
       <c r="L12" s="70"/>
     </row>
-    <row r="13" spans="1:12" s="18" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="18" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="69"/>
       <c r="B13" s="70"/>
       <c r="C13" s="71"/>
@@ -13010,7 +13016,7 @@
       <c r="K13" s="72"/>
       <c r="L13" s="70"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="53">
         <v>5</v>
       </c>
@@ -13034,7 +13040,7 @@
       </c>
       <c r="L14" s="55"/>
     </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D15" s="36" t="s">
         <v>9</v>
       </c>
@@ -13054,7 +13060,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D16" s="36" t="s">
         <v>10</v>
       </c>
@@ -13074,7 +13080,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D17" s="36" t="s">
         <v>34</v>
       </c>
@@ -13094,7 +13100,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D18" s="36" t="s">
         <v>11</v>
       </c>
@@ -13114,7 +13120,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D19" s="36" t="s">
         <v>12</v>
       </c>
@@ -13134,7 +13140,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="69"/>
       <c r="B20" s="70"/>
       <c r="C20" s="71"/>
@@ -13158,7 +13164,7 @@
       </c>
       <c r="L20" s="70"/>
     </row>
-    <row r="21" spans="1:12" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="18" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="69"/>
       <c r="B21" s="70"/>
       <c r="C21" s="71"/>
@@ -13182,7 +13188,7 @@
       <c r="K21" s="72"/>
       <c r="L21" s="70"/>
     </row>
-    <row r="22" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="53">
         <v>6</v>
       </c>
@@ -13210,7 +13216,7 @@
       </c>
       <c r="L22" s="55"/>
     </row>
-    <row r="23" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D23" s="36" t="s">
         <v>9</v>
       </c>
@@ -13233,7 +13239,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="69"/>
       <c r="B24" s="70"/>
       <c r="C24" s="71"/>
@@ -13263,7 +13269,7 @@
       </c>
       <c r="L24" s="70"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="53">
         <v>7</v>
       </c>
@@ -13287,7 +13293,7 @@
       </c>
       <c r="L25" s="55"/>
     </row>
-    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D26" s="36" t="s">
         <v>4</v>
       </c>
@@ -13310,7 +13316,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D27" s="36" t="s">
         <v>3</v>
       </c>
@@ -13330,7 +13336,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="69"/>
       <c r="B28" s="70"/>
       <c r="C28" s="71"/>
@@ -13356,7 +13362,7 @@
       </c>
       <c r="L28" s="70"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="53"/>
       <c r="B29" s="55"/>
       <c r="C29" s="61"/>
@@ -13384,23 +13390,23 @@
       <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="115" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="110" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="111" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="112" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="110" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" style="111" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.1640625" style="113" customWidth="1"/>
-    <col min="8" max="8" width="23.83203125" style="114" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.1640625" style="113" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="112" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="110" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" style="111" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="112" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="110" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1796875" style="111" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.1796875" style="113" customWidth="1"/>
+    <col min="8" max="8" width="23.81640625" style="114" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.1796875" style="113" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.36328125" style="112" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="112" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" style="110" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.36328125" style="110" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -13438,7 +13444,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -13472,7 +13478,7 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>2</v>
       </c>
@@ -13492,7 +13498,7 @@
       <c r="K3" s="54"/>
       <c r="L3" s="55"/>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="35"/>
       <c r="B4" s="41"/>
       <c r="C4" s="42"/>
@@ -13520,7 +13526,7 @@
       </c>
       <c r="L4" s="37"/>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="35"/>
       <c r="B5" s="37"/>
       <c r="C5" s="43"/>
@@ -13550,7 +13556,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="69"/>
       <c r="B6" s="70"/>
       <c r="C6" s="71"/>
@@ -13576,7 +13582,7 @@
       </c>
       <c r="L6" s="70"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="53">
         <v>3</v>
       </c>
@@ -13598,7 +13604,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="35"/>
       <c r="B8" s="41"/>
       <c r="C8" s="42"/>
@@ -13620,7 +13626,7 @@
       <c r="K8" s="36"/>
       <c r="L8" s="49"/>
     </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="35"/>
       <c r="B9" s="37"/>
       <c r="C9" s="43"/>
@@ -13642,7 +13648,7 @@
       <c r="K9" s="36"/>
       <c r="L9" s="37"/>
     </row>
-    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="69"/>
       <c r="B10" s="70"/>
       <c r="C10" s="71"/>
@@ -13666,7 +13672,7 @@
       <c r="K10" s="89"/>
       <c r="L10" s="90"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="53">
         <v>4</v>
       </c>
@@ -13690,7 +13696,7 @@
       </c>
       <c r="L11" s="55"/>
     </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="35"/>
       <c r="B12" s="41"/>
       <c r="C12" s="42"/>
@@ -13716,7 +13722,7 @@
       </c>
       <c r="L12" s="37"/>
     </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="35"/>
       <c r="B13" s="37"/>
       <c r="C13" s="43"/>
@@ -13742,7 +13748,7 @@
       </c>
       <c r="L13" s="37"/>
     </row>
-    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="69"/>
       <c r="B14" s="70"/>
       <c r="C14" s="71"/>
@@ -13764,7 +13770,7 @@
       <c r="K14" s="72"/>
       <c r="L14" s="70"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="53">
         <v>5</v>
       </c>
@@ -13788,7 +13794,7 @@
       </c>
       <c r="L15" s="55"/>
     </row>
-    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="35"/>
       <c r="B16" s="41"/>
       <c r="C16" s="42"/>
@@ -13816,7 +13822,7 @@
       </c>
       <c r="L16" s="37"/>
     </row>
-    <row r="17" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="69"/>
       <c r="B17" s="70"/>
       <c r="C17" s="71"/>
@@ -13844,7 +13850,7 @@
       </c>
       <c r="L17" s="70"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="53">
         <v>6</v>
       </c>
@@ -13868,7 +13874,7 @@
       </c>
       <c r="L18" s="55"/>
     </row>
-    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="35"/>
       <c r="B19" s="41"/>
       <c r="C19" s="42"/>
@@ -13894,7 +13900,7 @@
       </c>
       <c r="L19" s="37"/>
     </row>
-    <row r="20" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="35"/>
       <c r="B20" s="37"/>
       <c r="C20" s="43"/>
@@ -13920,7 +13926,7 @@
       </c>
       <c r="L20" s="37"/>
     </row>
-    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="35"/>
       <c r="B21" s="37"/>
       <c r="C21" s="43"/>
@@ -13946,7 +13952,7 @@
       </c>
       <c r="L21" s="37"/>
     </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="35"/>
       <c r="B22" s="37"/>
       <c r="C22" s="43"/>
@@ -13972,7 +13978,7 @@
       </c>
       <c r="L22" s="37"/>
     </row>
-    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="35"/>
       <c r="B23" s="37"/>
       <c r="C23" s="43"/>
@@ -13998,7 +14004,7 @@
       </c>
       <c r="L23" s="37"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="35"/>
       <c r="B24" s="37"/>
       <c r="C24" s="43"/>
@@ -14022,7 +14028,7 @@
       </c>
       <c r="L24" s="37"/>
     </row>
-    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="69"/>
       <c r="B25" s="70"/>
       <c r="C25" s="71"/>
@@ -14044,7 +14050,7 @@
       <c r="K25" s="72"/>
       <c r="L25" s="70"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="116" t="s">
         <v>322</v>
       </c>
@@ -14074,24 +14080,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.36328125" style="39" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.83203125" style="39" customWidth="1"/>
-    <col min="10" max="10" width="24.83203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.81640625" style="39" customWidth="1"/>
+    <col min="10" max="10" width="24.81640625" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="12" max="12" width="23.453125" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -14129,7 +14135,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -14161,7 +14167,7 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>2</v>
       </c>
@@ -14183,7 +14189,7 @@
       <c r="K3" s="54"/>
       <c r="L3" s="55"/>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B4" s="41"/>
       <c r="C4" s="42"/>
       <c r="D4" s="36" t="s">
@@ -14205,7 +14211,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D5" s="36" t="s">
         <v>61</v>
       </c>
@@ -14225,7 +14231,7 @@
         <v>3014</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
@@ -14245,7 +14251,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>34</v>
       </c>
@@ -14265,7 +14271,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D8" s="36" t="s">
         <v>87</v>
       </c>
@@ -14285,7 +14291,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D9" s="36" t="s">
         <v>174</v>
       </c>
@@ -14305,7 +14311,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D10" s="36" t="s">
         <v>14</v>
       </c>
@@ -14325,7 +14331,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="69"/>
       <c r="B11" s="70"/>
       <c r="C11" s="71"/>
@@ -14351,7 +14357,7 @@
       </c>
       <c r="L11" s="70"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="53">
         <v>3</v>
       </c>
@@ -14375,7 +14381,7 @@
       </c>
       <c r="L12" s="55"/>
     </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D13" s="36">
         <v>1</v>
       </c>
@@ -14395,7 +14401,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D14" s="36">
         <v>2</v>
       </c>
@@ -14415,7 +14421,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D15" s="36">
         <v>3</v>
       </c>
@@ -14438,7 +14444,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="69"/>
       <c r="B16" s="70"/>
       <c r="C16" s="71"/>
@@ -14462,7 +14468,7 @@
       <c r="K16" s="72"/>
       <c r="L16" s="70"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="53">
         <v>4</v>
       </c>
@@ -14486,7 +14492,7 @@
       </c>
       <c r="L17" s="55"/>
     </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D18" s="36" t="s">
         <v>5</v>
       </c>
@@ -14509,7 +14515,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D19" s="36" t="s">
         <v>6</v>
       </c>
@@ -14532,7 +14538,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="69"/>
       <c r="B20" s="70"/>
       <c r="C20" s="71"/>
@@ -14556,7 +14562,7 @@
       <c r="K20" s="72"/>
       <c r="L20" s="70"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="53">
         <v>5</v>
       </c>
@@ -14580,7 +14586,7 @@
       </c>
       <c r="L21" s="55"/>
     </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D22" s="36" t="s">
         <v>8</v>
       </c>
@@ -14600,7 +14606,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D23" s="36" t="s">
         <v>4</v>
       </c>
@@ -14623,7 +14629,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="69"/>
       <c r="B24" s="70"/>
       <c r="C24" s="71"/>
@@ -14645,7 +14651,7 @@
       <c r="K24" s="72"/>
       <c r="L24" s="70"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="53">
         <v>6</v>
       </c>
@@ -14669,7 +14675,7 @@
       </c>
       <c r="L25" s="55"/>
     </row>
-    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D26" s="36" t="s">
         <v>9</v>
       </c>
@@ -14689,7 +14695,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D27" s="36" t="s">
         <v>10</v>
       </c>
@@ -14709,7 +14715,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D28" s="36" t="s">
         <v>34</v>
       </c>
@@ -14729,7 +14735,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D29" s="36" t="s">
         <v>11</v>
       </c>
@@ -14749,7 +14755,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="69"/>
       <c r="B30" s="70"/>
       <c r="C30" s="71"/>
@@ -14775,7 +14781,7 @@
       </c>
       <c r="L30" s="70"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="53">
         <v>7</v>
       </c>
@@ -14799,7 +14805,7 @@
       </c>
       <c r="L31" s="55"/>
     </row>
-    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D32" s="36" t="s">
         <v>9</v>
       </c>
@@ -14819,7 +14825,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="69"/>
       <c r="B33" s="70"/>
       <c r="C33" s="71"/>
@@ -14849,7 +14855,7 @@
       </c>
       <c r="L33" s="70"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="53"/>
       <c r="B34" s="55"/>
       <c r="C34" s="61"/>
@@ -14877,24 +14883,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="43" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6328125" style="37" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="47.1640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="12" max="12" width="47.1796875" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>394</v>
       </c>
@@ -14932,7 +14938,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -14964,7 +14970,7 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>2</v>
       </c>
@@ -14984,7 +14990,7 @@
       <c r="K3" s="54"/>
       <c r="L3" s="55"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D4" s="36" t="s">
         <v>14</v>
       </c>
@@ -15004,7 +15010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D5" s="36" t="s">
         <v>4</v>
       </c>
@@ -15024,7 +15030,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>3</v>
       </c>
@@ -15044,7 +15050,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>8</v>
       </c>
@@ -15064,7 +15070,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="69"/>
       <c r="B8" s="70"/>
       <c r="C8" s="71"/>
@@ -15088,7 +15094,7 @@
       <c r="K8" s="72"/>
       <c r="L8" s="70"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="53">
         <v>3</v>
       </c>
@@ -15110,7 +15116,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D10" s="36" t="s">
         <v>174</v>
       </c>
@@ -15124,7 +15130,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D11" s="36" t="s">
         <v>5</v>
       </c>
@@ -15138,7 +15144,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D12" s="36" t="s">
         <v>4</v>
       </c>
@@ -15152,7 +15158,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D13" s="36" t="s">
         <v>78</v>
       </c>
@@ -15166,7 +15172,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="69"/>
       <c r="B14" s="70"/>
       <c r="C14" s="71"/>
@@ -15188,7 +15194,7 @@
       <c r="K14" s="72"/>
       <c r="L14" s="70"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="53"/>
       <c r="B15" s="55"/>
       <c r="C15" s="61"/>
@@ -15216,24 +15222,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" style="43" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.81640625" style="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="43" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.1640625" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.6328125" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.1796875" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.36328125" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="9"/>
+    <col min="12" max="12" width="23.36328125" style="37" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="83" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="122" t="s">
         <v>394</v>
       </c>
@@ -15271,7 +15277,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>1</v>
       </c>
@@ -15303,7 +15309,7 @@
       </c>
       <c r="L2" s="22"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="53">
         <v>2</v>
       </c>
@@ -15327,7 +15333,7 @@
       </c>
       <c r="L3" s="55"/>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D4" s="36" t="s">
         <v>4</v>
       </c>
@@ -15347,7 +15353,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="69"/>
       <c r="B5" s="70"/>
       <c r="C5" s="71"/>
@@ -15373,7 +15379,7 @@
       </c>
       <c r="L5" s="70"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="53">
         <v>3</v>
       </c>
@@ -15397,7 +15403,7 @@
       </c>
       <c r="L6" s="55"/>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>8</v>
       </c>
@@ -15420,7 +15426,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D8" s="36" t="s">
         <v>4</v>
       </c>
@@ -15443,7 +15449,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="69"/>
       <c r="B9" s="70"/>
       <c r="C9" s="71"/>
@@ -15467,7 +15473,7 @@
       <c r="K9" s="72"/>
       <c r="L9" s="70"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="53">
         <v>4</v>
       </c>
@@ -15493,7 +15499,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D11" s="36" t="s">
         <v>10</v>
       </c>
@@ -15510,7 +15516,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D12" s="36" t="s">
         <v>34</v>
       </c>
@@ -15527,7 +15533,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D13" s="36" t="s">
         <v>11</v>
       </c>
@@ -15541,7 +15547,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="69"/>
       <c r="B14" s="70"/>
       <c r="C14" s="71"/>
@@ -15565,7 +15571,7 @@
       <c r="K14" s="72"/>
       <c r="L14" s="70"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="53"/>
       <c r="B15" s="55"/>
       <c r="C15" s="61"/>

</xml_diff>

<commit_message>
Tagset changes for adverbs, new data
</commit_message>
<xml_diff>
--- a/docs/SemTi-Kamols_morphotags.xlsx
+++ b/docs/SemTi-Kamols_morphotags.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20396"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!LaumasDoc\Git\Treebank\Docs\Annotation how-to\Tags&amp;tagset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F51632-0BA4-47B4-8B7B-EE9AC85FF195}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5948A022-73BF-448C-949C-F02FE80A9FD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="31500" windowHeight="20740" tabRatio="725" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="31500" windowHeight="20740" tabRatio="725" firstSheet="10" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par|About" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1671" uniqueCount="799">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="804">
   <si>
     <t>Latviešu valodas morfoloģisko pazīmju kopa</t>
   </si>
@@ -3698,9 +3698,6 @@
     </r>
   </si>
   <si>
-    <t>relatīvais</t>
-  </si>
-  <si>
     <t>cēloņa/nolūka</t>
   </si>
   <si>
@@ -5647,6 +5644,48 @@
   </si>
   <si>
     <t>Syntactic function</t>
+  </si>
+  <si>
+    <t>Prepositional adverb</t>
+  </si>
+  <si>
+    <r>
+      <t>y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>es</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>o</t>
+    </r>
+  </si>
+  <si>
+    <t>labi, tad, vakar</t>
+  </si>
+  <si>
+    <t>Prievārdiskais apstākļa vārds</t>
+  </si>
+  <si>
+    <t>2023-03-23 Apstākļa vārdiem vērtību r no 2. pozīcijas izņem un izveido jaunu pozīciju tam.</t>
   </si>
 </sst>
 </file>
@@ -5868,7 +5907,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -5960,11 +5999,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -6431,6 +6490,36 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6811,12 +6900,12 @@
     </row>
     <row r="3" spans="2:4" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B3" s="20" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -6825,7 +6914,7 @@
         <v>54</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
@@ -6833,12 +6922,12 @@
         <v>0</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C9" s="5"/>
     </row>
@@ -6847,7 +6936,7 @@
         <v>300</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.35">
@@ -6855,7 +6944,7 @@
         <v>300</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
   </sheetData>
@@ -6868,7 +6957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
@@ -6901,7 +6990,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -6913,13 +7002,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="66" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="67" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -6942,10 +7031,10 @@
         <v>3</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="29"/>
@@ -6965,10 +7054,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="59" t="s">
+        <v>796</v>
+      </c>
+      <c r="C3" s="60" t="s">
         <v>797</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>798</v>
       </c>
       <c r="D3" s="54"/>
       <c r="E3" s="55"/>
@@ -6985,10 +7074,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H4" s="40" t="s">
         <v>232</v>
@@ -7008,10 +7097,10 @@
         <v>8</v>
       </c>
       <c r="E5" s="70" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F5" s="77" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="G5" s="74"/>
       <c r="H5" s="75" t="s">
@@ -7083,7 +7172,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -7095,13 +7184,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="68" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="64" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -7124,14 +7213,14 @@
         <v>87</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="28" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I2" s="22" t="s">
         <v>356</v>
@@ -7200,7 +7289,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -7212,13 +7301,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="68" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="64" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -7241,14 +7330,14 @@
         <v>174</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>275</v>
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="28" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="I2" s="22" t="s">
         <v>356</v>
@@ -7317,7 +7406,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -7329,13 +7418,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="68" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="64" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -7358,7 +7447,7 @@
         <v>276</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>277</v>
@@ -7405,10 +7494,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H4" s="36" t="s">
         <v>279</v>
@@ -7425,10 +7514,10 @@
         <v>174</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="H5" s="36" t="s">
         <v>281</v>
@@ -7448,16 +7537,16 @@
         <v>8</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="H6" s="36" t="s">
         <v>283</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="J6" s="36" t="s">
         <v>284</v>
@@ -7474,16 +7563,16 @@
         <v>286</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="F7" s="38" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="H7" s="36" t="s">
         <v>287</v>
       </c>
       <c r="I7" s="37" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="J7" s="40" t="s">
         <v>294</v>
@@ -7500,16 +7589,16 @@
         <v>34</v>
       </c>
       <c r="E8" s="124" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F8" s="38" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="H8" s="36" t="s">
         <v>289</v>
       </c>
       <c r="I8" s="37" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="J8" s="36" t="s">
         <v>290</v>
@@ -7523,13 +7612,13 @@
         <v>68</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F9" s="38" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="H9" s="36" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="J9" s="36" t="s">
         <v>291</v>
@@ -7549,13 +7638,13 @@
         <v>292</v>
       </c>
       <c r="F10" s="77" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G10" s="74" t="s">
         <v>293</v>
       </c>
       <c r="H10" s="75" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="I10" s="70"/>
       <c r="J10" s="72"/>
@@ -7619,7 +7708,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -7631,13 +7720,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="68" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="64" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -7660,10 +7749,10 @@
         <v>59</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G2" s="22" t="s">
         <v>296</v>
@@ -7696,10 +7785,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="55" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F3" s="56" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G3" s="55" t="s">
         <v>299</v>
@@ -7723,7 +7812,7 @@
         <v>401</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G4" s="37" t="s">
         <v>298</v>
@@ -7744,10 +7833,10 @@
         <v>11</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G5" s="37"/>
       <c r="H5" s="36" t="s">
@@ -7766,10 +7855,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="124" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G6" s="37"/>
       <c r="H6" s="36" t="s">
@@ -7788,10 +7877,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="129" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F7" s="132" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G7" s="129"/>
       <c r="H7" s="131" t="s">
@@ -7810,10 +7899,10 @@
         <v>34</v>
       </c>
       <c r="E8" s="139" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="F8" s="140" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G8" s="136"/>
       <c r="H8" s="138" t="s">
@@ -7881,7 +7970,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -7893,13 +7982,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="68" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="64" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -7922,7 +8011,7 @@
         <v>61</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F2" s="26" t="s">
         <v>302</v>
@@ -7932,7 +8021,7 @@
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="22" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>302</v>
@@ -7956,10 +8045,10 @@
         <v>6</v>
       </c>
       <c r="E3" s="55" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="F3" s="87" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G3" s="57" t="s">
         <v>310</v>
@@ -7977,7 +8066,7 @@
         <v>68</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F4" s="44" t="s">
         <v>556</v>
@@ -7994,16 +8083,16 @@
         <v>9</v>
       </c>
       <c r="E5" s="37" t="s">
+        <v>787</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>666</v>
+      </c>
+      <c r="G5" s="39" t="s">
         <v>788</v>
       </c>
-      <c r="F5" s="43" t="s">
-        <v>667</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>789</v>
-      </c>
       <c r="H5" s="40" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -8014,7 +8103,7 @@
         <v>306</v>
       </c>
       <c r="F6" s="38" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G6" s="39" t="s">
         <v>307</v>
@@ -8035,11 +8124,11 @@
         <v>292</v>
       </c>
       <c r="F7" s="71" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G7" s="74"/>
       <c r="H7" s="72" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="I7" s="70"/>
       <c r="J7" s="72"/>
@@ -8069,9 +8158,11 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -8091,9 +8182,9 @@
     <col min="14" max="16384" width="8.81640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="18"/>
@@ -8108,7 +8199,7 @@
       <c r="L1" s="18"/>
       <c r="M1" s="18"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -8127,7 +8218,7 @@
       <c r="L2" s="18"/>
       <c r="M2" s="18"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8146,15 +8237,15 @@
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B4" s="157"/>
     </row>
-    <row r="5" spans="1:14" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A5" s="142" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B5" s="17"/>
       <c r="C5" s="18"/>
@@ -8169,682 +8260,667 @@
       <c r="L5" s="18"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B6" s="157"/>
     </row>
-    <row r="7" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B7" s="157"/>
     </row>
-    <row r="8" spans="1:14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="141" t="s">
+        <v>803</v>
+      </c>
       <c r="B8" s="157"/>
     </row>
-    <row r="9" spans="1:14" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="142" t="s">
-        <v>670</v>
-      </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-    </row>
-    <row r="10" spans="1:14" s="143" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="145" t="s">
+    <row r="9" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="157"/>
+    </row>
+    <row r="10" spans="1:13" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="142" t="s">
+        <v>669</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+    </row>
+    <row r="11" spans="1:13" s="143" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="145" t="s">
         <v>406</v>
       </c>
-      <c r="B10" s="122" t="s">
+      <c r="B11" s="122" t="s">
         <v>394</v>
       </c>
-      <c r="C10" s="146" t="s">
+      <c r="C11" s="146" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="147" t="s">
+      <c r="D11" s="147" t="s">
         <v>396</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E11" s="66" t="s">
+        <v>732</v>
+      </c>
+      <c r="F11" s="64" t="s">
+        <v>398</v>
+      </c>
+      <c r="G11" s="65" t="s">
+        <v>397</v>
+      </c>
+      <c r="H11" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="68" t="s">
+        <v>729</v>
+      </c>
+      <c r="J11" s="67" t="s">
+        <v>348</v>
+      </c>
+      <c r="K11" s="68" t="s">
         <v>733</v>
       </c>
-      <c r="F10" s="64" t="s">
-        <v>398</v>
-      </c>
-      <c r="G10" s="65" t="s">
-        <v>397</v>
-      </c>
-      <c r="H10" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" s="68" t="s">
-        <v>730</v>
-      </c>
-      <c r="J10" s="67" t="s">
-        <v>348</v>
-      </c>
-      <c r="K10" s="68" t="s">
-        <v>734</v>
-      </c>
-      <c r="L10" s="68" t="s">
+      <c r="L11" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="64" t="s">
+      <c r="M11" s="64" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
+    <row r="12" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B12" s="27">
         <v>3</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D12" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E12" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="159" t="s">
+      <c r="F12" s="159" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G12" s="25" t="s">
         <v>407</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H12" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="I11" s="29" t="s">
+      <c r="I12" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="23"/>
-      <c r="K11" s="28" t="s">
+      <c r="J12" s="23"/>
+      <c r="K12" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="L11" s="28">
+      <c r="L12" s="28">
         <v>1558</v>
       </c>
-      <c r="M11" s="22" t="s">
+      <c r="M12" s="22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B12" s="53">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B13" s="53">
         <v>5</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C13" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="61" t="s">
+      <c r="D13" s="61" t="s">
         <v>423</v>
       </c>
-      <c r="E12" s="54" t="s">
+      <c r="E13" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="55" t="s">
+      <c r="F13" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="61" t="s">
+      <c r="G13" s="61" t="s">
         <v>433</v>
       </c>
-      <c r="H12" s="57" t="s">
+      <c r="H13" s="57" t="s">
         <v>329</v>
       </c>
-      <c r="I12" s="58" t="s">
+      <c r="I13" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="J12" s="57"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="55" t="s">
+      <c r="J13" s="57"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="54"/>
+      <c r="M13" s="55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="69"/>
-      <c r="C13" s="102"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="107"/>
-      <c r="F13" s="102"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="102"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="107"/>
-      <c r="L13" s="107"/>
-      <c r="M13" s="102"/>
-    </row>
-    <row r="14" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B14" s="69"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="107"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="107"/>
+      <c r="L14" s="107"/>
+      <c r="M14" s="102"/>
+    </row>
+    <row r="15" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
         <v>454</v>
       </c>
-      <c r="B14" s="53">
+      <c r="B15" s="53">
         <v>2</v>
       </c>
-      <c r="C14" s="55" t="s">
+      <c r="C15" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D15" s="61" t="s">
         <v>391</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E15" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="57" t="s">
+      <c r="F15" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="61"/>
-      <c r="H14" s="57" t="s">
+      <c r="G15" s="61"/>
+      <c r="H15" s="57" t="s">
         <v>381</v>
       </c>
-      <c r="I14" s="58" t="s">
+      <c r="I15" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="J14" s="57"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="78" t="s">
+      <c r="J15" s="57"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="54"/>
+      <c r="M15" s="78" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="69"/>
-      <c r="C15" s="102"/>
-      <c r="D15" s="103"/>
-      <c r="E15" s="107"/>
-      <c r="F15" s="102"/>
-      <c r="G15" s="103"/>
-      <c r="H15" s="102"/>
-      <c r="I15" s="107"/>
-      <c r="J15" s="102"/>
-      <c r="K15" s="107"/>
-      <c r="L15" s="107"/>
-      <c r="M15" s="102"/>
-    </row>
-    <row r="16" spans="1:14" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B16" s="69"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="107"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="107"/>
+      <c r="L16" s="107"/>
+      <c r="M16" s="102"/>
+    </row>
+    <row r="17" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
         <v>519</v>
       </c>
-      <c r="B16" s="53">
+      <c r="B17" s="53">
         <v>2</v>
       </c>
-      <c r="C16" s="55" t="s">
+      <c r="C17" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D17" s="61" t="s">
         <v>391</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E17" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="57" t="s">
+      <c r="F17" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="61"/>
-      <c r="H16" s="57" t="s">
+      <c r="G17" s="61"/>
+      <c r="H17" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="I16" s="58" t="s">
+      <c r="I17" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="57"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="78" t="s">
+      <c r="J17" s="57"/>
+      <c r="K17" s="54"/>
+      <c r="L17" s="54"/>
+      <c r="M17" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="N16" s="9"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B17" s="69"/>
-      <c r="C17" s="102"/>
-      <c r="D17" s="103"/>
-      <c r="E17" s="107"/>
-      <c r="F17" s="102"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="102"/>
-      <c r="I17" s="107"/>
-      <c r="J17" s="102"/>
-      <c r="K17" s="107"/>
-      <c r="L17" s="107"/>
-      <c r="M17" s="102"/>
-    </row>
-    <row r="18" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B18" s="69"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="102"/>
+      <c r="I18" s="107"/>
+      <c r="J18" s="102"/>
+      <c r="K18" s="107"/>
+      <c r="L18" s="107"/>
+      <c r="M18" s="102"/>
+    </row>
+    <row r="19" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="14" t="s">
         <v>554</v>
       </c>
-      <c r="B18" s="53">
+      <c r="B19" s="53">
         <v>7</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C19" s="59" t="s">
         <v>116</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D19" s="60" t="s">
         <v>531</v>
       </c>
-      <c r="E18" s="54" t="s">
+      <c r="E19" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="55" t="s">
+      <c r="F19" s="55" t="s">
         <v>254</v>
       </c>
-      <c r="G18" s="61"/>
-      <c r="H18" s="57" t="s">
+      <c r="G19" s="61"/>
+      <c r="H19" s="57" t="s">
         <v>255</v>
       </c>
-      <c r="I18" s="58" t="s">
+      <c r="I19" s="58" t="s">
         <v>267</v>
       </c>
-      <c r="J18" s="57"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="78" t="s">
+      <c r="J19" s="57"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="78" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="C19" s="37"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="37" t="s">
-        <v>256</v>
-      </c>
-      <c r="G19" s="43"/>
-      <c r="H19" s="39" t="s">
-        <v>257</v>
-      </c>
-      <c r="I19" s="40" t="s">
-        <v>268</v>
-      </c>
-      <c r="J19" s="39"/>
-      <c r="K19" s="36"/>
-      <c r="L19" s="36"/>
-      <c r="M19" s="37"/>
-    </row>
-    <row r="20" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C20" s="37"/>
       <c r="D20" s="43"/>
       <c r="E20" s="36" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="F20" s="37" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G20" s="43"/>
       <c r="H20" s="39" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="I20" s="40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J20" s="39"/>
       <c r="K20" s="36"/>
       <c r="L20" s="36"/>
       <c r="M20" s="37"/>
     </row>
-    <row r="21" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="C21" s="37"/>
       <c r="D21" s="43"/>
       <c r="E21" s="36" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="F21" s="37" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G21" s="43"/>
       <c r="H21" s="39" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I21" s="40" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J21" s="39"/>
       <c r="K21" s="36"/>
       <c r="L21" s="36"/>
       <c r="M21" s="37"/>
     </row>
-    <row r="22" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="C22" s="37"/>
       <c r="D22" s="43"/>
       <c r="E22" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="39" t="s">
-        <v>262</v>
+        <v>8</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>260</v>
       </c>
       <c r="G22" s="43"/>
       <c r="H22" s="39" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="I22" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J22" s="39"/>
       <c r="K22" s="36"/>
       <c r="L22" s="36"/>
       <c r="M22" s="37"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="C23" s="37"/>
       <c r="D23" s="43"/>
       <c r="E23" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="37" t="s">
-        <v>264</v>
+        <v>78</v>
+      </c>
+      <c r="F23" s="39" t="s">
+        <v>262</v>
       </c>
       <c r="G23" s="43"/>
-      <c r="H23" s="39"/>
+      <c r="H23" s="39" t="s">
+        <v>263</v>
+      </c>
       <c r="I23" s="40" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="J23" s="39"/>
       <c r="K23" s="36"/>
       <c r="L23" s="36"/>
       <c r="M23" s="37"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C24" s="37"/>
       <c r="D24" s="43"/>
       <c r="E24" s="36" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F24" s="37" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G24" s="43"/>
       <c r="H24" s="39"/>
       <c r="I24" s="40" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J24" s="39"/>
       <c r="K24" s="36"/>
       <c r="L24" s="36"/>
       <c r="M24" s="37"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B25" s="69"/>
-      <c r="C25" s="102"/>
-      <c r="D25" s="103"/>
-      <c r="E25" s="107"/>
-      <c r="F25" s="102"/>
-      <c r="G25" s="103"/>
-      <c r="H25" s="102"/>
-      <c r="I25" s="107"/>
-      <c r="J25" s="102"/>
-      <c r="K25" s="107"/>
-      <c r="L25" s="107"/>
-      <c r="M25" s="102"/>
-    </row>
-    <row r="26" spans="1:13" s="144" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="16" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C25" s="37"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>265</v>
+      </c>
+      <c r="G25" s="43"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="40" t="s">
+        <v>265</v>
+      </c>
+      <c r="J25" s="39"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="37"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B26" s="69"/>
+      <c r="C26" s="102"/>
+      <c r="D26" s="103"/>
+      <c r="E26" s="107"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="103"/>
+      <c r="H26" s="102"/>
+      <c r="I26" s="107"/>
+      <c r="J26" s="102"/>
+      <c r="K26" s="107"/>
+      <c r="L26" s="107"/>
+      <c r="M26" s="102"/>
+    </row>
+    <row r="27" spans="1:14" s="144" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
         <v>564</v>
       </c>
-      <c r="B26" s="148">
+      <c r="B27" s="148">
         <v>8</v>
       </c>
-      <c r="C26" s="149" t="s">
+      <c r="C27" s="149" t="s">
         <v>565</v>
       </c>
-      <c r="D26" s="150"/>
-      <c r="E26" s="151" t="s">
+      <c r="D27" s="150"/>
+      <c r="E27" s="151" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="152" t="s">
+      <c r="F27" s="152" t="s">
         <v>566</v>
       </c>
-      <c r="G26" s="153"/>
-      <c r="H26" s="154" t="s">
+      <c r="G27" s="153"/>
+      <c r="H27" s="154" t="s">
         <v>193</v>
       </c>
-      <c r="I26" s="155" t="s">
+      <c r="I27" s="155" t="s">
         <v>183</v>
       </c>
-      <c r="J26" s="152"/>
-      <c r="K26" s="151"/>
-      <c r="L26" s="151"/>
-      <c r="M26" s="156"/>
-    </row>
-    <row r="27" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="C27" s="37"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="H27" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="I27" s="40" t="s">
-        <v>185</v>
-      </c>
-      <c r="J27" s="37"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="J27" s="152"/>
+      <c r="K27" s="151"/>
+      <c r="L27" s="151"/>
+      <c r="M27" s="156"/>
+    </row>
+    <row r="28" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="C28" s="37"/>
       <c r="D28" s="43"/>
-      <c r="E28" s="36">
-        <v>0</v>
+      <c r="E28" s="36" t="s">
+        <v>8</v>
       </c>
       <c r="F28" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="47"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
+        <v>184</v>
+      </c>
+      <c r="H28" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="I28" s="40" t="s">
+        <v>185</v>
+      </c>
       <c r="J28" s="37"/>
       <c r="K28" s="36"/>
       <c r="L28" s="36"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B29" s="69"/>
-      <c r="C29" s="102"/>
-      <c r="D29" s="103"/>
-      <c r="E29" s="107"/>
-      <c r="F29" s="102"/>
-      <c r="G29" s="103"/>
-      <c r="H29" s="102"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="102"/>
-      <c r="K29" s="107"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="102"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="14" t="s">
-        <v>598</v>
-      </c>
-      <c r="B30" s="53">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C29" s="37"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="36">
+        <v>0</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="G29" s="47"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B30" s="69"/>
+      <c r="C30" s="102"/>
+      <c r="D30" s="103"/>
+      <c r="E30" s="107"/>
+      <c r="F30" s="102"/>
+      <c r="G30" s="103"/>
+      <c r="H30" s="102"/>
+      <c r="I30" s="107"/>
+      <c r="J30" s="102"/>
+      <c r="K30" s="107"/>
+      <c r="L30" s="107"/>
+      <c r="M30" s="102"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A31" s="14" t="s">
+        <v>597</v>
+      </c>
+      <c r="B31" s="53">
         <v>5</v>
       </c>
-      <c r="C30" s="59" t="s">
+      <c r="C31" s="59" t="s">
         <v>218</v>
       </c>
-      <c r="D30" s="79"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="123"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="82"/>
-      <c r="M30" s="78"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C31" s="37"/>
-      <c r="E31" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="F31" s="37" t="s">
-        <v>629</v>
-      </c>
-      <c r="G31" s="38" t="s">
-        <v>631</v>
-      </c>
-      <c r="I31" s="40" t="s">
-        <v>208</v>
-      </c>
-      <c r="J31" s="37"/>
-      <c r="K31" s="36"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D31" s="79"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="123"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="78"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C32" s="37"/>
       <c r="E32" s="36" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="F32" s="37" t="s">
+        <v>628</v>
+      </c>
+      <c r="G32" s="38" t="s">
         <v>630</v>
       </c>
-      <c r="G32" s="38" t="s">
-        <v>632</v>
-      </c>
       <c r="I32" s="40" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="J32" s="37"/>
       <c r="K32" s="36"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B33" s="69"/>
-      <c r="C33" s="102"/>
-      <c r="D33" s="103"/>
-      <c r="E33" s="107"/>
-      <c r="F33" s="102"/>
-      <c r="G33" s="103"/>
-      <c r="H33" s="102"/>
-      <c r="I33" s="107"/>
-      <c r="J33" s="102"/>
-      <c r="K33" s="107"/>
-      <c r="L33" s="107"/>
-      <c r="M33" s="102"/>
+      <c r="C33" s="37"/>
+      <c r="E33" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="37" t="s">
+        <v>629</v>
+      </c>
+      <c r="G33" s="38" t="s">
+        <v>631</v>
+      </c>
+      <c r="I33" s="40" t="s">
+        <v>219</v>
+      </c>
+      <c r="J33" s="37"/>
+      <c r="K33" s="36"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="14" t="s">
-        <v>611</v>
-      </c>
-      <c r="B34" s="53">
+      <c r="B34" s="69"/>
+      <c r="C34" s="102"/>
+      <c r="D34" s="103"/>
+      <c r="E34" s="107"/>
+      <c r="F34" s="102"/>
+      <c r="G34" s="103"/>
+      <c r="H34" s="102"/>
+      <c r="I34" s="107"/>
+      <c r="J34" s="102"/>
+      <c r="K34" s="107"/>
+      <c r="L34" s="107"/>
+      <c r="M34" s="102"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="14" t="s">
+        <v>610</v>
+      </c>
+      <c r="B35" s="53">
         <v>3</v>
       </c>
-      <c r="C34" s="59" t="s">
+      <c r="C35" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="D34" s="60" t="s">
-        <v>628</v>
-      </c>
-      <c r="E34" s="54"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="55" t="s">
+      <c r="D35" s="60" t="s">
+        <v>627</v>
+      </c>
+      <c r="E35" s="54"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="55" t="s">
         <v>324</v>
       </c>
-      <c r="I34" s="54"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="54"/>
-      <c r="L34" s="54"/>
-      <c r="M34" s="55"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="36" t="s">
+      <c r="I35" s="54"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="54"/>
+      <c r="L35" s="54"/>
+      <c r="M35" s="55"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C36" s="41"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="37" t="s">
+      <c r="F36" s="37" t="s">
         <v>561</v>
       </c>
-      <c r="G35" s="38" t="s">
-        <v>624</v>
-      </c>
-      <c r="H35" s="39"/>
-      <c r="I35" s="40" t="s">
-        <v>230</v>
-      </c>
-      <c r="J35" s="39"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="36"/>
-      <c r="M35" s="49" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C36" s="37"/>
-      <c r="D36" s="43"/>
-      <c r="E36" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F36" s="37" t="s">
-        <v>621</v>
-      </c>
       <c r="G36" s="38" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="H36" s="39"/>
       <c r="I36" s="40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J36" s="39"/>
       <c r="K36" s="36"/>
       <c r="L36" s="36"/>
-      <c r="M36" s="37"/>
-    </row>
-    <row r="37" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="M36" s="49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C37" s="37"/>
       <c r="D37" s="43"/>
       <c r="E37" s="36" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="F37" s="37" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="G37" s="38" t="s">
-        <v>626</v>
-      </c>
-      <c r="H37" s="113" t="s">
-        <v>233</v>
-      </c>
+        <v>624</v>
+      </c>
+      <c r="H37" s="39"/>
       <c r="I37" s="40" t="s">
-        <v>323</v>
+        <v>231</v>
       </c>
       <c r="J37" s="39"/>
       <c r="K37" s="36"/>
       <c r="L37" s="36"/>
       <c r="M37" s="37"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C38" s="37"/>
       <c r="D38" s="43"/>
       <c r="E38" s="36" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="F38" s="37" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="G38" s="38" t="s">
-        <v>627</v>
-      </c>
-      <c r="H38" s="39"/>
+        <v>625</v>
+      </c>
+      <c r="H38" s="113" t="s">
+        <v>233</v>
+      </c>
       <c r="I38" s="40" t="s">
-        <v>234</v>
+        <v>323</v>
       </c>
       <c r="J38" s="39"/>
       <c r="K38" s="36"/>
@@ -8852,221 +8928,242 @@
       <c r="M38" s="37"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B39" s="69"/>
-      <c r="C39" s="70"/>
-      <c r="D39" s="71"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="70"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="74"/>
-      <c r="I39" s="75"/>
-      <c r="J39" s="74"/>
-      <c r="K39" s="72"/>
-      <c r="L39" s="72"/>
-      <c r="M39" s="70"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="37" t="s">
+        <v>622</v>
+      </c>
+      <c r="G39" s="38" t="s">
+        <v>626</v>
+      </c>
+      <c r="H39" s="39"/>
+      <c r="I39" s="40" t="s">
+        <v>234</v>
+      </c>
+      <c r="J39" s="39"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="36"/>
+      <c r="M39" s="37"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A40" s="14" t="s">
-        <v>620</v>
-      </c>
-      <c r="B40" s="53">
+      <c r="B40" s="69"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="77"/>
+      <c r="H40" s="74"/>
+      <c r="I40" s="75"/>
+      <c r="J40" s="74"/>
+      <c r="K40" s="72"/>
+      <c r="L40" s="72"/>
+      <c r="M40" s="70"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41" s="14" t="s">
+        <v>619</v>
+      </c>
+      <c r="B41" s="53">
         <v>2</v>
       </c>
-      <c r="C40" s="59" t="s">
+      <c r="C41" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="D40" s="60" t="s">
-        <v>628</v>
-      </c>
-      <c r="E40" s="54"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="55"/>
-      <c r="I40" s="54"/>
-      <c r="J40" s="55"/>
-      <c r="K40" s="54"/>
-      <c r="L40" s="54"/>
-      <c r="M40" s="78" t="s">
+      <c r="D41" s="60" t="s">
+        <v>627</v>
+      </c>
+      <c r="E41" s="54"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="61"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="54"/>
+      <c r="L41" s="54"/>
+      <c r="M41" s="78" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="36" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C42" s="41"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="37" t="s">
+      <c r="F42" s="37" t="s">
         <v>561</v>
       </c>
-      <c r="G41" s="38" t="s">
-        <v>624</v>
-      </c>
-      <c r="H41" s="37"/>
-      <c r="I41" s="36" t="s">
+      <c r="G42" s="38" t="s">
+        <v>623</v>
+      </c>
+      <c r="H42" s="37"/>
+      <c r="I42" s="36" t="s">
         <v>273</v>
-      </c>
-      <c r="J41" s="37"/>
-      <c r="K41" s="36"/>
-      <c r="L41" s="36"/>
-    </row>
-    <row r="42" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="C42" s="37"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F42" s="37" t="s">
-        <v>621</v>
-      </c>
-      <c r="G42" s="38" t="s">
-        <v>625</v>
-      </c>
-      <c r="H42" s="37"/>
-      <c r="I42" s="40" t="s">
-        <v>274</v>
       </c>
       <c r="J42" s="37"/>
       <c r="K42" s="36"/>
       <c r="L42" s="36"/>
-      <c r="M42" s="37"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B43" s="69"/>
-      <c r="C43" s="102"/>
-      <c r="D43" s="103"/>
-      <c r="E43" s="107"/>
-      <c r="F43" s="102"/>
-      <c r="G43" s="103"/>
-      <c r="H43" s="102"/>
-      <c r="I43" s="107"/>
-      <c r="J43" s="102"/>
-      <c r="K43" s="107"/>
-      <c r="L43" s="107"/>
-      <c r="M43" s="102"/>
+    </row>
+    <row r="43" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="C43" s="37"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F43" s="37" t="s">
+        <v>620</v>
+      </c>
+      <c r="G43" s="38" t="s">
+        <v>624</v>
+      </c>
+      <c r="H43" s="37"/>
+      <c r="I43" s="40" t="s">
+        <v>274</v>
+      </c>
+      <c r="J43" s="37"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="36"/>
+      <c r="M43" s="37"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="14" t="s">
-        <v>634</v>
-      </c>
-      <c r="B44" s="53">
+      <c r="B44" s="69"/>
+      <c r="C44" s="102"/>
+      <c r="D44" s="103"/>
+      <c r="E44" s="107"/>
+      <c r="F44" s="102"/>
+      <c r="G44" s="103"/>
+      <c r="H44" s="102"/>
+      <c r="I44" s="107"/>
+      <c r="J44" s="102"/>
+      <c r="K44" s="107"/>
+      <c r="L44" s="107"/>
+      <c r="M44" s="102"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45" s="14" t="s">
+        <v>633</v>
+      </c>
+      <c r="B45" s="53">
         <v>2</v>
       </c>
-      <c r="C44" s="59" t="s">
+      <c r="C45" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="D44" s="60" t="s">
-        <v>628</v>
-      </c>
-      <c r="E44" s="54"/>
-      <c r="F44" s="55"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="55"/>
-      <c r="I44" s="54"/>
-      <c r="J44" s="55"/>
-      <c r="K44" s="54"/>
-      <c r="L44" s="82"/>
-      <c r="M44" s="78" t="s">
+      <c r="D45" s="60" t="s">
+        <v>627</v>
+      </c>
+      <c r="E45" s="54"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="54"/>
+      <c r="L45" s="82"/>
+      <c r="M45" s="78" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="36" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C46" s="41"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="F45" s="37" t="s">
+      <c r="F46" s="37" t="s">
         <v>561</v>
       </c>
-      <c r="G45" s="38" t="s">
-        <v>624</v>
-      </c>
-      <c r="H45" s="37" t="s">
+      <c r="G46" s="38" t="s">
+        <v>623</v>
+      </c>
+      <c r="H46" s="37" t="s">
         <v>230</v>
-      </c>
-      <c r="I45" s="36"/>
-      <c r="J45" s="37"/>
-      <c r="K45" s="36"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C46" s="37"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F46" s="37" t="s">
-        <v>621</v>
-      </c>
-      <c r="G46" s="38" t="s">
-        <v>625</v>
-      </c>
-      <c r="H46" s="37" t="s">
-        <v>231</v>
       </c>
       <c r="I46" s="36"/>
       <c r="J46" s="37"/>
       <c r="K46" s="36"/>
-      <c r="L46" s="36"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B47" s="69"/>
-      <c r="C47" s="102"/>
-      <c r="D47" s="103"/>
-      <c r="E47" s="107"/>
-      <c r="F47" s="102"/>
-      <c r="G47" s="103"/>
-      <c r="H47" s="102"/>
-      <c r="I47" s="107"/>
-      <c r="J47" s="102"/>
-      <c r="K47" s="107"/>
-      <c r="L47" s="107"/>
-      <c r="M47" s="102"/>
-    </row>
-    <row r="48" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="14" t="s">
-        <v>669</v>
-      </c>
-      <c r="B48" s="27">
+      <c r="C47" s="37"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F47" s="37" t="s">
+        <v>620</v>
+      </c>
+      <c r="G47" s="38" t="s">
+        <v>624</v>
+      </c>
+      <c r="H47" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="I47" s="36"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="36"/>
+      <c r="L47" s="36"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B48" s="69"/>
+      <c r="C48" s="102"/>
+      <c r="D48" s="103"/>
+      <c r="E48" s="107"/>
+      <c r="F48" s="102"/>
+      <c r="G48" s="103"/>
+      <c r="H48" s="102"/>
+      <c r="I48" s="107"/>
+      <c r="J48" s="102"/>
+      <c r="K48" s="107"/>
+      <c r="L48" s="107"/>
+      <c r="M48" s="102"/>
+    </row>
+    <row r="49" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="14" t="s">
+        <v>668</v>
+      </c>
+      <c r="B49" s="27">
         <v>2</v>
       </c>
-      <c r="C48" s="22" t="s">
+      <c r="C49" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D48" s="26" t="s">
+      <c r="D49" s="26" t="s">
         <v>391</v>
       </c>
-      <c r="E48" s="160" t="s">
+      <c r="E49" s="160" t="s">
         <v>78</v>
       </c>
-      <c r="F48" s="161" t="s">
-        <v>666</v>
-      </c>
-      <c r="G48" s="162" t="s">
+      <c r="F49" s="161" t="s">
         <v>665</v>
       </c>
-      <c r="H48" s="163" t="s">
-        <v>731</v>
-      </c>
-      <c r="I48" s="164"/>
-      <c r="J48" s="165"/>
-      <c r="K48" s="160"/>
-      <c r="L48" s="160"/>
-      <c r="M48" s="161"/>
-    </row>
-    <row r="49" spans="2:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="53"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="79"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="78"/>
-      <c r="G49" s="79"/>
-      <c r="H49" s="78"/>
-      <c r="I49" s="82"/>
-      <c r="J49" s="78"/>
-      <c r="K49" s="82"/>
-      <c r="L49" s="82"/>
-      <c r="M49" s="78"/>
+      <c r="G49" s="162" t="s">
+        <v>664</v>
+      </c>
+      <c r="H49" s="163" t="s">
+        <v>730</v>
+      </c>
+      <c r="I49" s="164"/>
+      <c r="J49" s="165"/>
+      <c r="K49" s="160"/>
+      <c r="L49" s="160"/>
+      <c r="M49" s="161"/>
+    </row>
+    <row r="50" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="53"/>
+      <c r="C50" s="78"/>
+      <c r="D50" s="79"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="78"/>
+      <c r="G50" s="79"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="82"/>
+      <c r="J50" s="78"/>
+      <c r="K50" s="82"/>
+      <c r="L50" s="82"/>
+      <c r="M50" s="78"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9079,7 +9176,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
@@ -9111,7 +9208,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -9123,13 +9220,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="66" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="67" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -9335,10 +9432,10 @@
         <v>408</v>
       </c>
       <c r="G9" s="74" t="s">
+        <v>759</v>
+      </c>
+      <c r="H9" s="75" t="s">
         <v>760</v>
-      </c>
-      <c r="H9" s="75" t="s">
-        <v>761</v>
       </c>
       <c r="I9" s="74"/>
       <c r="J9" s="72"/>
@@ -9383,7 +9480,7 @@
       </c>
       <c r="G11" s="39"/>
       <c r="H11" s="40" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="I11" s="39"/>
       <c r="J11" s="36" t="s">
@@ -9408,7 +9505,7 @@
       </c>
       <c r="G12" s="39"/>
       <c r="H12" s="40" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="I12" s="39"/>
       <c r="J12" s="36" t="s">
@@ -9656,7 +9753,7 @@
       </c>
       <c r="G22" s="39"/>
       <c r="H22" s="40" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="I22" s="39"/>
       <c r="J22" s="36" t="s">
@@ -9874,10 +9971,10 @@
       </c>
       <c r="G32" s="39"/>
       <c r="H32" s="40" t="s">
+        <v>757</v>
+      </c>
+      <c r="I32" s="39" t="s">
         <v>758</v>
-      </c>
-      <c r="I32" s="39" t="s">
-        <v>759</v>
       </c>
       <c r="J32" s="36"/>
       <c r="K32" s="36"/>
@@ -9966,7 +10063,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -9978,13 +10075,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="66" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="67" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -10161,16 +10258,16 @@
         <v>78</v>
       </c>
       <c r="E9" s="74" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F9" s="76" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G9" s="74" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="H9" s="75" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="I9" s="74"/>
       <c r="J9" s="72" t="s">
@@ -10180,7 +10277,7 @@
         <v>1244</v>
       </c>
       <c r="L9" s="74" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -10191,16 +10288,16 @@
         <v>11</v>
       </c>
       <c r="E10" s="74" t="s">
+        <v>766</v>
+      </c>
+      <c r="F10" s="76" t="s">
+        <v>762</v>
+      </c>
+      <c r="G10" s="74" t="s">
+        <v>770</v>
+      </c>
+      <c r="H10" s="75" t="s">
         <v>767</v>
-      </c>
-      <c r="F10" s="76" t="s">
-        <v>763</v>
-      </c>
-      <c r="G10" s="74" t="s">
-        <v>771</v>
-      </c>
-      <c r="H10" s="75" t="s">
-        <v>768</v>
       </c>
       <c r="I10" s="74"/>
       <c r="J10" s="72" t="s">
@@ -10210,7 +10307,7 @@
         <v>1244</v>
       </c>
       <c r="L10" s="74" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -10286,10 +10383,10 @@
         <v>49</v>
       </c>
       <c r="F14" s="94" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="G14" s="92" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="H14" s="93"/>
       <c r="I14" s="92"/>
@@ -10391,10 +10488,10 @@
         <v>470</v>
       </c>
       <c r="G19" s="39" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H19" s="40" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="L19" s="49" t="s">
         <v>53</v>
@@ -10502,7 +10599,7 @@
         <v>479</v>
       </c>
       <c r="H24" s="40" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="J24" s="36" t="s">
         <v>102</v>
@@ -10522,7 +10619,7 @@
         <v>480</v>
       </c>
       <c r="H25" s="40" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="J25" s="36" t="s">
         <v>103</v>
@@ -10542,7 +10639,7 @@
         <v>481</v>
       </c>
       <c r="H26" s="40" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="J26" s="36" t="s">
         <v>104</v>
@@ -10640,10 +10737,10 @@
         <v>49</v>
       </c>
       <c r="F31" s="71" t="s">
+        <v>670</v>
+      </c>
+      <c r="G31" s="74" t="s">
         <v>671</v>
-      </c>
-      <c r="G31" s="74" t="s">
-        <v>672</v>
       </c>
       <c r="H31" s="75"/>
       <c r="I31" s="74"/>
@@ -10686,7 +10783,7 @@
         <v>486</v>
       </c>
       <c r="H33" s="40" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.35">
@@ -10700,7 +10797,7 @@
         <v>488</v>
       </c>
       <c r="H34" s="40" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.35">
@@ -10714,7 +10811,7 @@
         <v>490</v>
       </c>
       <c r="H35" s="40" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.35">
@@ -10745,10 +10842,10 @@
         <v>49</v>
       </c>
       <c r="F37" s="71" t="s">
+        <v>670</v>
+      </c>
+      <c r="G37" s="74" t="s">
         <v>671</v>
-      </c>
-      <c r="G37" s="74" t="s">
-        <v>672</v>
       </c>
       <c r="H37" s="75"/>
       <c r="I37" s="74"/>
@@ -10791,7 +10888,7 @@
         <v>494</v>
       </c>
       <c r="H39" s="40" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.35">
@@ -10805,7 +10902,7 @@
         <v>496</v>
       </c>
       <c r="H40" s="40" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.35">
@@ -10819,7 +10916,7 @@
         <v>498</v>
       </c>
       <c r="H41" s="40" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -10879,7 +10976,7 @@
         <v>409</v>
       </c>
       <c r="H44" s="40" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="J44" s="36" t="s">
         <v>32</v>
@@ -10899,7 +10996,7 @@
         <v>410</v>
       </c>
       <c r="H45" s="40" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="J45" s="36" t="s">
         <v>33</v>
@@ -10981,10 +11078,10 @@
         <v>507</v>
       </c>
       <c r="F49" s="44" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="G49" s="39" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J49" s="36" t="s">
         <v>119</v>
@@ -11031,7 +11128,7 @@
       <c r="G51" s="57"/>
       <c r="H51" s="58"/>
       <c r="I51" s="57" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="J51" s="54" t="s">
         <v>121</v>
@@ -11114,7 +11211,7 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -11146,7 +11243,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -11158,13 +11255,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="66" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="67" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -11324,7 +11421,7 @@
         <v>76</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="J8" s="36" t="s">
         <v>77</v>
@@ -11341,16 +11438,16 @@
         <v>78</v>
       </c>
       <c r="E9" s="74" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F9" s="76" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G9" s="74" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="H9" s="166" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="I9" s="74"/>
       <c r="J9" s="72" t="s">
@@ -11360,7 +11457,7 @@
         <v>1244</v>
       </c>
       <c r="L9" s="74" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
@@ -11371,16 +11468,16 @@
         <v>11</v>
       </c>
       <c r="E10" s="74" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F10" s="76" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="G10" s="74" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="H10" s="166" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="I10" s="74"/>
       <c r="J10" s="72" t="s">
@@ -11390,7 +11487,7 @@
         <v>1244</v>
       </c>
       <c r="L10" s="74" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -11466,10 +11563,10 @@
         <v>49</v>
       </c>
       <c r="F14" s="91" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="G14" s="92" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="H14" s="93"/>
       <c r="I14" s="92"/>
@@ -11947,10 +12044,10 @@
         <v>528</v>
       </c>
       <c r="G34" s="105" t="s">
+        <v>776</v>
+      </c>
+      <c r="H34" s="106" t="s">
         <v>777</v>
-      </c>
-      <c r="H34" s="106" t="s">
-        <v>778</v>
       </c>
       <c r="I34" s="105"/>
       <c r="J34" s="107"/>
@@ -12020,7 +12117,7 @@
       </c>
       <c r="G37" s="48"/>
       <c r="H37" s="51" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="I37" s="48"/>
       <c r="J37" s="52" t="s">
@@ -12045,7 +12142,7 @@
       </c>
       <c r="G38" s="48"/>
       <c r="H38" s="51" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="I38" s="48"/>
       <c r="J38" s="52" t="s">
@@ -12070,7 +12167,7 @@
       </c>
       <c r="G39" s="48"/>
       <c r="H39" s="51" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="I39" s="48"/>
       <c r="J39" s="52" t="s">
@@ -12095,7 +12192,7 @@
       </c>
       <c r="G40" s="48"/>
       <c r="H40" s="51" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="I40" s="48"/>
       <c r="J40" s="52" t="s">
@@ -12193,7 +12290,7 @@
         <v>142</v>
       </c>
       <c r="H44" s="51" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="I44" s="48"/>
       <c r="J44" s="52" t="s">
@@ -12220,7 +12317,7 @@
         <v>143</v>
       </c>
       <c r="H45" s="51" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="I45" s="48"/>
       <c r="J45" s="52" t="s">
@@ -12295,7 +12392,7 @@
         <v>144</v>
       </c>
       <c r="H48" s="51" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="I48" s="48"/>
       <c r="J48" s="52" t="s">
@@ -12322,7 +12419,7 @@
         <v>145</v>
       </c>
       <c r="H49" s="51" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="I49" s="48"/>
       <c r="J49" s="52" t="s">
@@ -12587,7 +12684,7 @@
       <c r="G60" s="57"/>
       <c r="H60" s="58"/>
       <c r="I60" s="57" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="J60" s="54" t="s">
         <v>121</v>
@@ -12671,7 +12768,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -12703,7 +12800,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -12715,13 +12812,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="66" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="67" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -12752,7 +12849,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="29"/>
       <c r="I2" s="23" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>152</v>
@@ -12817,7 +12914,7 @@
       </c>
       <c r="G5" s="74"/>
       <c r="H5" s="75" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I5" s="74"/>
       <c r="J5" s="72"/>
@@ -12840,7 +12937,7 @@
       <c r="E6" s="55"/>
       <c r="F6" s="61"/>
       <c r="G6" s="57" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="H6" s="58" t="s">
         <v>167</v>
@@ -12865,7 +12962,7 @@
         <v>390</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="J7" s="36" t="s">
         <v>24</v>
@@ -12889,7 +12986,7 @@
       </c>
       <c r="G8" s="74"/>
       <c r="H8" s="75" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I8" s="74"/>
       <c r="J8" s="72" t="s">
@@ -12914,10 +13011,10 @@
         <v>408</v>
       </c>
       <c r="G9" s="74" t="s">
+        <v>793</v>
+      </c>
+      <c r="H9" s="75" t="s">
         <v>794</v>
-      </c>
-      <c r="H9" s="75" t="s">
-        <v>795</v>
       </c>
       <c r="I9" s="74"/>
       <c r="J9" s="72"/>
@@ -12959,7 +13056,7 @@
         <v>409</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="J11" s="36" t="s">
         <v>32</v>
@@ -12983,7 +13080,7 @@
       </c>
       <c r="G12" s="74"/>
       <c r="H12" s="75" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="I12" s="74"/>
       <c r="J12" s="72" t="s">
@@ -13006,10 +13103,10 @@
       </c>
       <c r="F13" s="71"/>
       <c r="G13" s="74" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H13" s="75" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="I13" s="74"/>
       <c r="J13" s="72"/>
@@ -13051,7 +13148,7 @@
         <v>417</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="J15" s="36" t="s">
         <v>155</v>
@@ -13071,7 +13168,7 @@
         <v>418</v>
       </c>
       <c r="H16" s="40" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="J16" s="36" t="s">
         <v>156</v>
@@ -13091,7 +13188,7 @@
         <v>419</v>
       </c>
       <c r="H17" s="40" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="J17" s="36" t="s">
         <v>157</v>
@@ -13111,7 +13208,7 @@
         <v>427</v>
       </c>
       <c r="H18" s="40" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="J18" s="36" t="s">
         <v>158</v>
@@ -13131,7 +13228,7 @@
         <v>428</v>
       </c>
       <c r="H19" s="40" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="J19" s="36" t="s">
         <v>159</v>
@@ -13181,7 +13278,7 @@
         <v>313</v>
       </c>
       <c r="H21" s="75" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="I21" s="74"/>
       <c r="J21" s="72"/>
@@ -13202,10 +13299,10 @@
       <c r="E22" s="55"/>
       <c r="F22" s="61"/>
       <c r="G22" s="57" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="H22" s="58" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="I22" s="57"/>
       <c r="J22" s="54" t="s">
@@ -13227,10 +13324,10 @@
         <v>534</v>
       </c>
       <c r="H23" s="40" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="I23" s="39" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="J23" s="36" t="s">
         <v>149</v>
@@ -13253,13 +13350,13 @@
         <v>535</v>
       </c>
       <c r="G24" s="74" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H24" s="75" t="s">
+        <v>745</v>
+      </c>
+      <c r="I24" s="74" t="s">
         <v>746</v>
-      </c>
-      <c r="I24" s="74" t="s">
-        <v>747</v>
       </c>
       <c r="J24" s="72" t="s">
         <v>151</v>
@@ -13304,7 +13401,7 @@
         <v>536</v>
       </c>
       <c r="G26" s="39" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="H26" s="40" t="s">
         <v>163</v>
@@ -13327,7 +13424,7 @@
         <v>539</v>
       </c>
       <c r="H27" s="40" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="J27" s="36" t="s">
         <v>165</v>
@@ -13351,7 +13448,7 @@
       </c>
       <c r="G28" s="74"/>
       <c r="H28" s="75" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="I28" s="74"/>
       <c r="J28" s="72" t="s">
@@ -13386,7 +13483,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -13417,7 +13514,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -13429,13 +13526,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="66" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="67" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -13468,7 +13565,7 @@
       </c>
       <c r="H2" s="29"/>
       <c r="I2" s="23" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>235</v>
@@ -13659,10 +13756,10 @@
         <v>563</v>
       </c>
       <c r="F10" s="94" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G10" s="92" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="H10" s="93" t="s">
         <v>248</v>
@@ -13837,7 +13934,7 @@
       </c>
       <c r="G17" s="74"/>
       <c r="H17" s="75" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="I17" s="74" t="s">
         <v>580</v>
@@ -13889,7 +13986,7 @@
       </c>
       <c r="G19" s="39"/>
       <c r="H19" s="40" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="I19" s="39"/>
       <c r="J19" s="36" t="s">
@@ -13915,7 +14012,7 @@
       </c>
       <c r="G20" s="39"/>
       <c r="H20" s="40" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="I20" s="39"/>
       <c r="J20" s="36" t="s">
@@ -13941,7 +14038,7 @@
       </c>
       <c r="G21" s="39"/>
       <c r="H21" s="40" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I21" s="39"/>
       <c r="J21" s="36" t="s">
@@ -13967,7 +14064,7 @@
       </c>
       <c r="G22" s="39"/>
       <c r="H22" s="40" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="I22" s="39"/>
       <c r="J22" s="36" t="s">
@@ -13993,7 +14090,7 @@
       </c>
       <c r="G23" s="39"/>
       <c r="H23" s="40" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I23" s="39"/>
       <c r="J23" s="36" t="s">
@@ -14076,7 +14173,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -14108,7 +14205,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -14120,13 +14217,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="66" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="67" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -14202,7 +14299,7 @@
         <v>569</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="J4" s="36" t="s">
         <v>169</v>
@@ -14222,7 +14319,7 @@
         <v>570</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="J5" s="36" t="s">
         <v>170</v>
@@ -14242,7 +14339,7 @@
         <v>571</v>
       </c>
       <c r="H6" s="40" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J6" s="36" t="s">
         <v>171</v>
@@ -14282,7 +14379,7 @@
         <v>573</v>
       </c>
       <c r="H8" s="40" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="J8" s="36" t="s">
         <v>173</v>
@@ -14302,7 +14399,7 @@
         <v>574</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J9" s="36" t="s">
         <v>175</v>
@@ -14322,7 +14419,7 @@
         <v>468</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J10" s="36" t="s">
         <v>176</v>
@@ -14392,7 +14489,7 @@
         <v>494</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J13" s="36" t="s">
         <v>178</v>
@@ -14412,7 +14509,7 @@
         <v>496</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="J14" s="36" t="s">
         <v>179</v>
@@ -14435,7 +14532,7 @@
         <v>187</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="J15" s="36" t="s">
         <v>180</v>
@@ -14503,7 +14600,7 @@
         <v>390</v>
       </c>
       <c r="H18" s="40" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="I18" s="39" t="s">
         <v>353</v>
@@ -14526,7 +14623,7 @@
         <v>403</v>
       </c>
       <c r="H19" s="40" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I19" s="39" t="s">
         <v>354</v>
@@ -14597,7 +14694,7 @@
         <v>409</v>
       </c>
       <c r="H22" s="40" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="J22" s="36" t="s">
         <v>32</v>
@@ -14617,7 +14714,7 @@
         <v>410</v>
       </c>
       <c r="H23" s="40" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I23" s="39" t="s">
         <v>355</v>
@@ -14686,7 +14783,7 @@
         <v>417</v>
       </c>
       <c r="H26" s="40" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="J26" s="36" t="s">
         <v>155</v>
@@ -14706,7 +14803,7 @@
         <v>418</v>
       </c>
       <c r="H27" s="40" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="J27" s="36" t="s">
         <v>156</v>
@@ -14726,7 +14823,7 @@
         <v>419</v>
       </c>
       <c r="H28" s="40" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="J28" s="36" t="s">
         <v>157</v>
@@ -14746,7 +14843,7 @@
         <v>427</v>
       </c>
       <c r="H29" s="40" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="J29" s="36" t="s">
         <v>158</v>
@@ -14770,7 +14867,7 @@
       </c>
       <c r="G30" s="74"/>
       <c r="H30" s="75" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I30" s="74"/>
       <c r="J30" s="72" t="s">
@@ -14816,7 +14913,7 @@
         <v>510</v>
       </c>
       <c r="H32" s="40" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="J32" s="36" t="s">
         <v>81</v>
@@ -14876,18 +14973,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="43" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" style="37" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" style="43" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.453125" style="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.81640625" style="37" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.453125" style="43" bestFit="1" customWidth="1"/>
@@ -14911,7 +15008,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -14923,13 +15020,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="66" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="64" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -14960,7 +15057,7 @@
       <c r="G2" s="22"/>
       <c r="H2" s="28"/>
       <c r="I2" s="23" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="J2" s="28" t="s">
         <v>195</v>
@@ -14992,133 +15089,127 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D4" s="36" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>588</v>
+        <v>548</v>
       </c>
       <c r="F4" s="38" t="s">
-        <v>546</v>
-      </c>
-      <c r="G4" s="37" t="s">
-        <v>196</v>
+        <v>585</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="49" t="s">
-        <v>53</v>
+        <v>379</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="K4" s="36">
+        <v>1420</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D5" s="36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F5" s="38" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="J5" s="36" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K5" s="36">
-        <v>1420</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>550</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>587</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>377</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="K6" s="36">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="72">
+        <v>0</v>
+      </c>
+      <c r="E7" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="71" t="s">
+        <v>466</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>375</v>
+      </c>
+      <c r="H7" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="I7" s="70"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="70"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" s="53">
         <v>3</v>
       </c>
-      <c r="E6" s="37" t="s">
-        <v>549</v>
-      </c>
-      <c r="F6" s="38" t="s">
-        <v>586</v>
-      </c>
-      <c r="H6" s="36" t="s">
-        <v>378</v>
-      </c>
-      <c r="J6" s="36" t="s">
-        <v>165</v>
-      </c>
-      <c r="K6" s="36">
-        <v>1421</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D7" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>550</v>
-      </c>
-      <c r="F7" s="38" t="s">
-        <v>587</v>
-      </c>
-      <c r="H7" s="36" t="s">
-        <v>377</v>
-      </c>
-      <c r="J7" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="K7" s="36">
-        <v>1422</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8" s="69"/>
-      <c r="B8" s="70"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="72">
-        <v>0</v>
-      </c>
-      <c r="E8" s="70" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="71" t="s">
-        <v>466</v>
-      </c>
-      <c r="G8" s="70" t="s">
-        <v>375</v>
-      </c>
-      <c r="H8" s="72" t="s">
-        <v>376</v>
-      </c>
-      <c r="I8" s="70"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="70"/>
+      <c r="B8" s="59" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="60" t="s">
+        <v>581</v>
+      </c>
+      <c r="D8" s="54"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="55" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9" s="53">
-        <v>3</v>
-      </c>
-      <c r="B9" s="59" t="s">
-        <v>197</v>
-      </c>
-      <c r="C9" s="60" t="s">
-        <v>581</v>
-      </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="55"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="55" t="s">
-        <v>198</v>
+      <c r="D9" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>593</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>589</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D10" s="36" t="s">
-        <v>174</v>
+        <v>5</v>
       </c>
       <c r="E10" s="37" t="s">
         <v>594</v>
@@ -15127,12 +15218,12 @@
         <v>590</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D11" s="36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>595</v>
@@ -15141,12 +15232,12 @@
         <v>591</v>
       </c>
       <c r="H11" s="36" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D12" s="36" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>596</v>
@@ -15155,61 +15246,110 @@
         <v>592</v>
       </c>
       <c r="H12" s="36" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="D13" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>597</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>593</v>
-      </c>
-      <c r="H13" s="36" t="s">
-        <v>202</v>
-      </c>
+      <c r="A13" s="69"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="70" t="s">
+        <v>588</v>
+      </c>
+      <c r="F13" s="77" t="s">
+        <v>584</v>
+      </c>
+      <c r="G13" s="70"/>
+      <c r="H13" s="72" t="s">
+        <v>203</v>
+      </c>
+      <c r="I13" s="70"/>
+      <c r="J13" s="72"/>
+      <c r="K13" s="72"/>
+      <c r="L13" s="70"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14" s="69"/>
-      <c r="B14" s="70"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="72" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="70" t="s">
-        <v>589</v>
-      </c>
-      <c r="F14" s="77" t="s">
-        <v>584</v>
-      </c>
-      <c r="G14" s="70"/>
-      <c r="H14" s="72" t="s">
-        <v>203</v>
-      </c>
-      <c r="I14" s="70"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="70"/>
+      <c r="A14" s="53">
+        <v>4</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>802</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>798</v>
+      </c>
+      <c r="D14" s="54"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="55"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" s="53"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="55"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="55"/>
+      <c r="D15" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>465</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>799</v>
+      </c>
+      <c r="G15" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="H15" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="176" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="171"/>
+      <c r="B16" s="172"/>
+      <c r="C16" s="173"/>
+      <c r="D16" s="174" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="172" t="s">
+        <v>463</v>
+      </c>
+      <c r="F16" s="175" t="s">
+        <v>800</v>
+      </c>
+      <c r="G16" s="172"/>
+      <c r="H16" s="174" t="s">
+        <v>801</v>
+      </c>
+      <c r="I16" s="172"/>
+      <c r="J16" s="174"/>
+      <c r="K16" s="174"/>
+      <c r="L16" s="172"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="167"/>
+      <c r="B17" s="168"/>
+      <c r="C17" s="169"/>
+      <c r="D17" s="170"/>
+      <c r="E17" s="168"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="168"/>
+      <c r="H17" s="170"/>
+      <c r="I17" s="168"/>
+      <c r="J17" s="170"/>
+      <c r="K17" s="170"/>
+      <c r="L17" s="168"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15250,7 +15390,7 @@
         <v>396</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E1" s="64" t="s">
         <v>398</v>
@@ -15262,13 +15402,13 @@
         <v>52</v>
       </c>
       <c r="H1" s="66" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I1" s="67" t="s">
         <v>348</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="K1" s="68" t="s">
         <v>16</v>
@@ -15291,10 +15431,10 @@
         <v>8</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="29"/>
@@ -15317,7 +15457,7 @@
         <v>204</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D3" s="54"/>
       <c r="E3" s="55"/>
@@ -15338,10 +15478,10 @@
         <v>4</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F4" s="86" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="H4" s="40" t="s">
         <v>205</v>
@@ -15361,10 +15501,10 @@
         <v>78</v>
       </c>
       <c r="E5" s="70" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F5" s="76" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G5" s="74"/>
       <c r="H5" s="75" t="s">
@@ -15387,7 +15527,7 @@
         <v>30</v>
       </c>
       <c r="C6" s="60" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D6" s="54"/>
       <c r="E6" s="55"/>
@@ -15460,7 +15600,7 @@
         <v>49</v>
       </c>
       <c r="F9" s="76" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G9" s="74" t="s">
         <v>220</v>
@@ -15481,7 +15621,7 @@
         <v>212</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D10" s="54"/>
       <c r="E10" s="55"/>
@@ -15507,7 +15647,7 @@
         <v>38</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G11" s="39" t="s">
         <v>215</v>
@@ -15524,7 +15664,7 @@
         <v>40</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G12" s="39" t="s">
         <v>224</v>
@@ -15558,7 +15698,7 @@
         <v>49</v>
       </c>
       <c r="F14" s="76" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G14" s="74" t="s">
         <v>220</v>

</xml_diff>

<commit_message>
Updates for pronoun loading from tezaurs
</commit_message>
<xml_diff>
--- a/docs/SemTi-Kamols_morphotags.xlsx
+++ b/docs/SemTi-Kamols_morphotags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!LaumasDoc\Git\Treebank\Docs\Annotation how-to\Tags&amp;tagset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7550BD-CBD3-4827-9BAC-49A0C3A730CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7F375D-0FFF-4676-AC19-DE555F616960}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="31500" windowHeight="20740" tabRatio="725" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="31500" windowHeight="20740" tabRatio="725" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par|About" sheetId="1" r:id="rId1"/>
@@ -5616,9 +5616,6 @@
     <t>sakrīt ar formu</t>
   </si>
   <si>
-    <t>15, 10 000 000, +371 29 787 121, XVII, MDCCCLXXXVIII</t>
-  </si>
-  <si>
     <t>normalizē uz ascii</t>
   </si>
   <si>
@@ -6852,6 +6849,9 @@
   </si>
   <si>
     <t>Apstākļa vārds</t>
+  </si>
+  <si>
+    <t>15, 10 000 000, +371 29 787 121, XVII, MDCCCLXXXVIII, 10.12.1999</t>
   </si>
 </sst>
 </file>
@@ -8129,18 +8129,18 @@
     </row>
     <row r="5" spans="2:4" ht="72.5">
       <c r="B5" s="182" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C5" s="184" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="183" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C6" s="177" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="8" spans="2:4">
@@ -8162,7 +8162,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="12" spans="2:4">
@@ -8221,7 +8221,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -8237,7 +8237,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -8326,10 +8326,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="59" t="s">
+        <v>791</v>
+      </c>
+      <c r="C5" s="60" t="s">
         <v>792</v>
-      </c>
-      <c r="C5" s="60" t="s">
-        <v>793</v>
       </c>
       <c r="D5" s="54"/>
       <c r="E5" s="55"/>
@@ -8435,7 +8435,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -8451,7 +8451,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -8584,7 +8584,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -8600,7 +8600,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -8733,13 +8733,13 @@
   <sheetData>
     <row r="1" spans="1:12" s="18" customFormat="1">
       <c r="A1" s="18" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="G1" s="178"/>
     </row>
     <row r="2" spans="1:12" s="18" customFormat="1">
       <c r="A2" s="18" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="G2" s="178"/>
     </row>
@@ -8894,7 +8894,7 @@
         <v>283</v>
       </c>
       <c r="I8" s="37" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="J8" s="36" t="s">
         <v>284</v>
@@ -8920,7 +8920,7 @@
         <v>287</v>
       </c>
       <c r="I9" s="37" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="J9" s="40" t="s">
         <v>294</v>
@@ -8946,7 +8946,7 @@
         <v>289</v>
       </c>
       <c r="I10" s="37" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="J10" s="36" t="s">
         <v>290</v>
@@ -9047,7 +9047,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -9063,7 +9063,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -9317,9 +9317,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -9341,10 +9341,10 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -9359,7 +9359,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -9492,7 +9492,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="29">
+    <row r="7" spans="1:12" ht="43.5">
       <c r="D7" s="36" t="s">
         <v>9</v>
       </c>
@@ -9506,7 +9506,7 @@
         <v>786</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>788</v>
+        <v>817</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -9688,13 +9688,13 @@
     </row>
     <row r="8" spans="1:13" customFormat="1">
       <c r="A8" s="141" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B8" s="157"/>
     </row>
     <row r="9" spans="1:13" customFormat="1">
       <c r="A9" s="141" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B9" s="157"/>
     </row>
@@ -10573,7 +10573,7 @@
     </row>
     <row r="51" spans="1:13" s="14" customFormat="1">
       <c r="A51" s="14" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B51" s="53">
         <v>3</v>
@@ -10750,10 +10750,10 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="18" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C1" s="178"/>
       <c r="D1" s="178"/>
@@ -10769,7 +10769,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="18" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="178"/>
@@ -11641,10 +11641,10 @@
   <sheetData>
     <row r="1" spans="1:12" s="18" customFormat="1">
       <c r="A1" s="18" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="H1" s="178"/>
       <c r="I1" s="178"/>
@@ -11652,7 +11652,7 @@
     </row>
     <row r="2" spans="1:12" s="18" customFormat="1">
       <c r="A2" s="18" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2" s="62"/>
       <c r="H2" s="178"/>
@@ -12841,10 +12841,10 @@
   <sheetData>
     <row r="1" spans="1:12" s="18" customFormat="1">
       <c r="A1" s="18" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="H1" s="178"/>
       <c r="I1" s="178"/>
@@ -12852,7 +12852,7 @@
     </row>
     <row r="2" spans="1:12" s="18" customFormat="1">
       <c r="A2" s="18" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="H2" s="178"/>
       <c r="I2" s="178"/>
@@ -14417,10 +14417,10 @@
   <sheetData>
     <row r="1" spans="1:12" s="18" customFormat="1">
       <c r="A1" s="18" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="H1" s="178"/>
       <c r="I1" s="178"/>
@@ -14428,7 +14428,7 @@
     </row>
     <row r="2" spans="1:12" s="18" customFormat="1">
       <c r="A2" s="18" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="H2" s="178"/>
       <c r="I2" s="178"/>
@@ -14656,10 +14656,10 @@
         <v>407</v>
       </c>
       <c r="G11" s="74" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="H11" s="75" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="I11" s="74"/>
       <c r="J11" s="72"/>
@@ -14748,10 +14748,10 @@
       </c>
       <c r="F15" s="71"/>
       <c r="G15" s="74" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="H15" s="75" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="I15" s="74"/>
       <c r="J15" s="72"/>
@@ -14923,7 +14923,7 @@
         <v>313</v>
       </c>
       <c r="H23" s="75" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="I23" s="74"/>
       <c r="J23" s="72"/>
@@ -15150,10 +15150,10 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -15168,7 +15168,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
@@ -15829,7 +15829,7 @@
     <row r="28" spans="1:12">
       <c r="A28" s="116"/>
       <c r="B28" s="181" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C28" s="118"/>
       <c r="D28" s="119"/>
@@ -15875,10 +15875,10 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -15893,7 +15893,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -16688,7 +16688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
@@ -16712,10 +16712,10 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -16730,7 +16730,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -16923,10 +16923,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="59" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C10" s="60" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D10" s="54"/>
       <c r="E10" s="55"/>
@@ -16946,7 +16946,7 @@
         <v>464</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="G11" s="37" t="s">
         <v>196</v>
@@ -16969,11 +16969,11 @@
         <v>462</v>
       </c>
       <c r="F12" s="175" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="G12" s="172"/>
       <c r="H12" s="174" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="I12" s="172"/>
       <c r="J12" s="174"/>
@@ -17028,7 +17028,7 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -17044,7 +17044,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>

</xml_diff>

<commit_message>
Drošības pēc jaunāks tagu excelis
</commit_message>
<xml_diff>
--- a/docs/SemTi-Kamols_morphotags.xlsx
+++ b/docs/SemTi-Kamols_morphotags.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!LaumasDoc\Git\Treebank\Docs\Annotation how-to\Tags&amp;tagset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A419C54-F607-4CD8-865D-1CAB3E33E998}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD30CD16-9913-4B89-B501-AC80D02575D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="31500" windowHeight="20740" tabRatio="725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="31500" windowHeight="20740" tabRatio="725" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Par|About" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="819">
   <si>
     <t>Latviešu valodas morfoloģisko pazīmju kopa</t>
   </si>
@@ -6493,19 +6493,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">nelokāms īpašības vārds, ja saskaņojas ar nelokāmu lietvārdu kam tēzaurā.lv nav norādīta dzimte vai ģenitīveni </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>(piemērs cukīni gan ir ar dzimti tēzaurā)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Apstākļa vārda pamatforma ir apstākļa vārda vienīgā forma (</t>
     </r>
     <r>
@@ -6852,13 +6839,19 @@
       </rPr>
       <t xml:space="preserve"> – siev. dz.). Tēzaurā neesošiem nelokāmiem personvārdiem (Eno) dzimti marķē pēc personas dzimuma, ja tas ir zināms. Nelokāmiem uzņēmumu nosaukumiem (Volvo) dzimte nepiemīt. Atšķirībā no tradicionālās gramatikas morfoloģisko pazīmju kopā nav lietots instrumentālis, jo tas vienskaitlī sakrīt ar akuzatīvu, bet daudzskaitlī – ar datīvu.</t>
     </r>
+  </si>
+  <si>
+    <t>mini (lietojumā mini kakao)</t>
+  </si>
+  <si>
+    <t>nelokāms īpašības vārds, ja saskaņojas ar nelokāmu lietvārdu kam tēzaurā.lv nav norādīta dzimte vai ģenitīveni</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7055,11 +7048,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="6">
@@ -8102,9 +8090,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.36328125" style="2" customWidth="1"/>
     <col min="2" max="2" width="13.36328125" style="2" customWidth="1"/>
@@ -8113,19 +8101,19 @@
     <col min="5" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1" ht="18.5">
+    <row r="2" spans="2:4" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1" ht="18.5">
+    <row r="3" spans="2:4" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B3" s="20" t="s">
         <v>723</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="72.5">
+    <row r="5" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B5" s="182" t="s">
         <v>804</v>
       </c>
@@ -8133,7 +8121,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="183" t="s">
         <v>805</v>
       </c>
@@ -8141,13 +8129,13 @@
         <v>799</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>720</v>
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>54</v>
       </c>
@@ -8155,7 +8143,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="8">
         <v>0</v>
       </c>
@@ -8163,13 +8151,13 @@
         <v>809</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="4" t="s">
         <v>726</v>
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="21" t="s">
         <v>300</v>
       </c>
@@ -8177,7 +8165,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
         <v>300</v>
       </c>
@@ -8200,7 +8188,7 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.36328125" style="37" bestFit="1" customWidth="1"/>
@@ -8217,7 +8205,7 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>804</v>
       </c>
@@ -8233,7 +8221,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>805</v>
       </c>
@@ -8249,7 +8237,7 @@
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -8287,7 +8275,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -8319,7 +8307,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>2</v>
       </c>
@@ -8339,7 +8327,7 @@
       <c r="K5" s="54"/>
       <c r="L5" s="55"/>
     </row>
-    <row r="6" spans="1:12" ht="43.5">
+    <row r="6" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>3</v>
       </c>
@@ -8359,7 +8347,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="69"/>
       <c r="B7" s="70"/>
       <c r="C7" s="71"/>
@@ -8385,7 +8373,7 @@
       </c>
       <c r="L7" s="70"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="53"/>
       <c r="B8" s="55"/>
       <c r="C8" s="61"/>
@@ -8414,7 +8402,7 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
@@ -8431,7 +8419,7 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>804</v>
       </c>
@@ -8447,7 +8435,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>805</v>
       </c>
@@ -8463,7 +8451,7 @@
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -8501,7 +8489,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -8535,7 +8523,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="53"/>
       <c r="B5" s="55"/>
       <c r="C5" s="61"/>
@@ -8563,7 +8551,7 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
@@ -8580,7 +8568,7 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>804</v>
       </c>
@@ -8596,7 +8584,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>805</v>
       </c>
@@ -8612,7 +8600,7 @@
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -8650,7 +8638,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -8684,7 +8672,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="53"/>
       <c r="B5" s="55"/>
       <c r="C5" s="61"/>
@@ -8712,7 +8700,7 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
@@ -8729,19 +8717,19 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="18" customFormat="1">
+    <row r="1" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>804</v>
       </c>
       <c r="G1" s="178"/>
     </row>
-    <row r="2" spans="1:12" s="18" customFormat="1">
+    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>805</v>
       </c>
       <c r="G2" s="178"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -8779,7 +8767,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -8813,7 +8801,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>2</v>
       </c>
@@ -8833,7 +8821,7 @@
       <c r="K5" s="54"/>
       <c r="L5" s="55"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6" s="41"/>
       <c r="C6" s="42"/>
       <c r="D6" s="36" t="s">
@@ -8855,7 +8843,7 @@
         <v>1448</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>174</v>
       </c>
@@ -8878,7 +8866,7 @@
         <v>2081</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D8" s="36" t="s">
         <v>8</v>
       </c>
@@ -8904,7 +8892,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="29">
+    <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D9" s="36" t="s">
         <v>286</v>
       </c>
@@ -8930,7 +8918,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D10" s="36" t="s">
         <v>34</v>
       </c>
@@ -8953,7 +8941,7 @@
         <v>2077</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D11" s="36" t="s">
         <v>68</v>
       </c>
@@ -8973,7 +8961,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="43.5">
+    <row r="12" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="69"/>
       <c r="B12" s="70"/>
       <c r="C12" s="71"/>
@@ -8997,7 +8985,7 @@
       <c r="K12" s="72"/>
       <c r="L12" s="70"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="53"/>
       <c r="B13" s="55"/>
       <c r="C13" s="61"/>
@@ -9026,7 +9014,7 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
@@ -9043,7 +9031,7 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>804</v>
       </c>
@@ -9059,7 +9047,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>805</v>
       </c>
@@ -9075,7 +9063,7 @@
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -9113,7 +9101,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -9149,7 +9137,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12" s="12" customFormat="1">
+    <row r="5" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>2</v>
       </c>
@@ -9179,7 +9167,7 @@
       <c r="K5" s="133"/>
       <c r="L5" s="134"/>
     </row>
-    <row r="6" spans="1:12" s="12" customFormat="1">
+    <row r="6" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="35"/>
       <c r="B6" s="37"/>
       <c r="C6" s="43"/>
@@ -9203,7 +9191,7 @@
       <c r="K6" s="126"/>
       <c r="L6" s="127"/>
     </row>
-    <row r="7" spans="1:12" s="12" customFormat="1">
+    <row r="7" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="35"/>
       <c r="B7" s="37"/>
       <c r="C7" s="43"/>
@@ -9225,7 +9213,7 @@
       <c r="K7" s="126"/>
       <c r="L7" s="127"/>
     </row>
-    <row r="8" spans="1:12" s="12" customFormat="1">
+    <row r="8" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="35"/>
       <c r="B8" s="37"/>
       <c r="C8" s="43"/>
@@ -9247,7 +9235,7 @@
       <c r="K8" s="126"/>
       <c r="L8" s="127"/>
     </row>
-    <row r="9" spans="1:12" s="125" customFormat="1">
+    <row r="9" spans="1:12" s="125" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="128"/>
       <c r="B9" s="129"/>
       <c r="C9" s="130"/>
@@ -9269,7 +9257,7 @@
       <c r="K9" s="131"/>
       <c r="L9" s="129"/>
     </row>
-    <row r="10" spans="1:12" s="125" customFormat="1">
+    <row r="10" spans="1:12" s="125" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="135"/>
       <c r="B10" s="136"/>
       <c r="C10" s="137"/>
@@ -9291,7 +9279,7 @@
       <c r="K10" s="138"/>
       <c r="L10" s="136"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="53"/>
       <c r="B11" s="55"/>
       <c r="C11" s="61"/>
@@ -9320,7 +9308,7 @@
       <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
@@ -9337,7 +9325,7 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>804</v>
       </c>
@@ -9355,7 +9343,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>805</v>
       </c>
@@ -9371,7 +9359,7 @@
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -9409,7 +9397,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -9443,7 +9431,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12" ht="29">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>2</v>
       </c>
@@ -9473,7 +9461,7 @@
       <c r="K5" s="54"/>
       <c r="L5" s="55"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>68</v>
       </c>
@@ -9490,7 +9478,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="43.5">
+    <row r="7" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>9</v>
       </c>
@@ -9504,10 +9492,10 @@
         <v>786</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D8" s="36" t="s">
         <v>135</v>
       </c>
@@ -9525,7 +9513,7 @@
       </c>
       <c r="I8" s="110"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="69"/>
       <c r="B9" s="70"/>
       <c r="C9" s="71"/>
@@ -9547,7 +9535,7 @@
       <c r="K9" s="72"/>
       <c r="L9" s="70"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="53"/>
       <c r="B10" s="55"/>
       <c r="C10" s="61"/>
@@ -9576,7 +9564,7 @@
       <selection activeCell="A56" sqref="A56:XFD56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" style="18" customWidth="1"/>
     <col min="2" max="2" width="2" style="35" bestFit="1" customWidth="1"/>
@@ -9594,7 +9582,7 @@
     <col min="14" max="16384" width="8.81640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>729</v>
       </c>
@@ -9611,7 +9599,7 @@
       <c r="L1" s="18"/>
       <c r="M1" s="18"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -9630,7 +9618,7 @@
       <c r="L2" s="18"/>
       <c r="M2" s="18"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9649,13 +9637,13 @@
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:13" customFormat="1">
+    <row r="4" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>722</v>
       </c>
       <c r="B4" s="157"/>
     </row>
-    <row r="5" spans="1:13" ht="18.5">
+    <row r="5" spans="1:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A5" s="142" t="s">
         <v>761</v>
       </c>
@@ -9672,34 +9660,34 @@
       <c r="L5" s="18"/>
       <c r="M5" s="18"/>
     </row>
-    <row r="6" spans="1:13" customFormat="1">
+    <row r="6" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>762</v>
       </c>
       <c r="B6" s="157"/>
     </row>
-    <row r="7" spans="1:13" customFormat="1">
+    <row r="7" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>779</v>
       </c>
       <c r="B7" s="157"/>
     </row>
-    <row r="8" spans="1:13" customFormat="1">
+    <row r="8" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="141" t="s">
         <v>798</v>
       </c>
       <c r="B8" s="157"/>
     </row>
-    <row r="9" spans="1:13" customFormat="1">
+    <row r="9" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="141" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="B9" s="157"/>
     </row>
-    <row r="10" spans="1:13" customFormat="1">
+    <row r="10" spans="1:13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="157"/>
     </row>
-    <row r="11" spans="1:13" ht="18.5">
+    <row r="11" spans="1:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A11" s="142" t="s">
         <v>668</v>
       </c>
@@ -9716,7 +9704,7 @@
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
     </row>
-    <row r="12" spans="1:13" s="143" customFormat="1" ht="29">
+    <row r="12" spans="1:13" s="143" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="145" t="s">
         <v>405</v>
       </c>
@@ -9757,7 +9745,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="29">
+    <row r="13" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>404</v>
       </c>
@@ -9796,7 +9784,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B14" s="53">
         <v>5</v>
       </c>
@@ -9828,7 +9816,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B15" s="69"/>
       <c r="C15" s="102"/>
       <c r="D15" s="103"/>
@@ -9842,7 +9830,7 @@
       <c r="L15" s="107"/>
       <c r="M15" s="102"/>
     </row>
-    <row r="16" spans="1:13" ht="43.5">
+    <row r="16" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>453</v>
       </c>
@@ -9875,7 +9863,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B17" s="69"/>
       <c r="C17" s="102"/>
       <c r="D17" s="103"/>
@@ -9889,7 +9877,7 @@
       <c r="L17" s="107"/>
       <c r="M17" s="102"/>
     </row>
-    <row r="18" spans="1:14" ht="29">
+    <row r="18" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="15" t="s">
         <v>518</v>
       </c>
@@ -9923,7 +9911,7 @@
       </c>
       <c r="N18" s="9"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B19" s="69"/>
       <c r="C19" s="102"/>
       <c r="D19" s="103"/>
@@ -9937,7 +9925,7 @@
       <c r="L19" s="107"/>
       <c r="M19" s="102"/>
     </row>
-    <row r="20" spans="1:14" ht="43.5">
+    <row r="20" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>553</v>
       </c>
@@ -9970,7 +9958,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="43.5">
+    <row r="21" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C21" s="37"/>
       <c r="D21" s="43"/>
       <c r="E21" s="36" t="s">
@@ -9991,7 +9979,7 @@
       <c r="L21" s="36"/>
       <c r="M21" s="37"/>
     </row>
-    <row r="22" spans="1:14" ht="29">
+    <row r="22" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="C22" s="37"/>
       <c r="D22" s="43"/>
       <c r="E22" s="36" t="s">
@@ -10012,7 +10000,7 @@
       <c r="L22" s="36"/>
       <c r="M22" s="37"/>
     </row>
-    <row r="23" spans="1:14" ht="29">
+    <row r="23" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="C23" s="37"/>
       <c r="D23" s="43"/>
       <c r="E23" s="36" t="s">
@@ -10033,7 +10021,7 @@
       <c r="L23" s="36"/>
       <c r="M23" s="37"/>
     </row>
-    <row r="24" spans="1:14" ht="29">
+    <row r="24" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="C24" s="37"/>
       <c r="D24" s="43"/>
       <c r="E24" s="36" t="s">
@@ -10054,7 +10042,7 @@
       <c r="L24" s="36"/>
       <c r="M24" s="37"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C25" s="37"/>
       <c r="D25" s="43"/>
       <c r="E25" s="36" t="s">
@@ -10073,7 +10061,7 @@
       <c r="L25" s="36"/>
       <c r="M25" s="37"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C26" s="37"/>
       <c r="D26" s="43"/>
       <c r="E26" s="36" t="s">
@@ -10092,7 +10080,7 @@
       <c r="L26" s="36"/>
       <c r="M26" s="37"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B27" s="69"/>
       <c r="C27" s="102"/>
       <c r="D27" s="103"/>
@@ -10106,7 +10094,7 @@
       <c r="L27" s="107"/>
       <c r="M27" s="102"/>
     </row>
-    <row r="28" spans="1:14" s="144" customFormat="1" ht="15.5">
+    <row r="28" spans="1:14" s="144" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="s">
         <v>563</v>
       </c>
@@ -10135,7 +10123,7 @@
       <c r="L28" s="151"/>
       <c r="M28" s="156"/>
     </row>
-    <row r="29" spans="1:14" ht="29">
+    <row r="29" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="C29" s="37"/>
       <c r="D29" s="43"/>
       <c r="E29" s="36" t="s">
@@ -10154,7 +10142,7 @@
       <c r="K29" s="36"/>
       <c r="L29" s="36"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C30" s="37"/>
       <c r="D30" s="43"/>
       <c r="E30" s="36">
@@ -10170,7 +10158,7 @@
       <c r="K30" s="36"/>
       <c r="L30" s="36"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B31" s="69"/>
       <c r="C31" s="102"/>
       <c r="D31" s="103"/>
@@ -10184,7 +10172,7 @@
       <c r="L31" s="107"/>
       <c r="M31" s="102"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
         <v>596</v>
       </c>
@@ -10205,7 +10193,7 @@
       <c r="L32" s="82"/>
       <c r="M32" s="78"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C33" s="37"/>
       <c r="E33" s="36" t="s">
         <v>59</v>
@@ -10222,7 +10210,7 @@
       <c r="J33" s="37"/>
       <c r="K33" s="36"/>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C34" s="37"/>
       <c r="E34" s="36" t="s">
         <v>9</v>
@@ -10239,7 +10227,7 @@
       <c r="J34" s="37"/>
       <c r="K34" s="36"/>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B35" s="69"/>
       <c r="C35" s="102"/>
       <c r="D35" s="103"/>
@@ -10253,7 +10241,7 @@
       <c r="L35" s="107"/>
       <c r="M35" s="102"/>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
         <v>609</v>
       </c>
@@ -10278,7 +10266,7 @@
       <c r="L36" s="54"/>
       <c r="M36" s="55"/>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C37" s="41"/>
       <c r="D37" s="42"/>
       <c r="E37" s="36" t="s">
@@ -10301,7 +10289,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C38" s="37"/>
       <c r="D38" s="43"/>
       <c r="E38" s="36" t="s">
@@ -10322,7 +10310,7 @@
       <c r="L38" s="36"/>
       <c r="M38" s="37"/>
     </row>
-    <row r="39" spans="1:13" ht="72.5">
+    <row r="39" spans="1:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C39" s="37"/>
       <c r="D39" s="43"/>
       <c r="E39" s="36" t="s">
@@ -10345,7 +10333,7 @@
       <c r="L39" s="36"/>
       <c r="M39" s="37"/>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C40" s="37"/>
       <c r="D40" s="43"/>
       <c r="E40" s="36" t="s">
@@ -10366,7 +10354,7 @@
       <c r="L40" s="36"/>
       <c r="M40" s="37"/>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B41" s="69"/>
       <c r="C41" s="70"/>
       <c r="D41" s="71"/>
@@ -10380,7 +10368,7 @@
       <c r="L41" s="72"/>
       <c r="M41" s="70"/>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="14" t="s">
         <v>618</v>
       </c>
@@ -10405,7 +10393,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C43" s="41"/>
       <c r="D43" s="42"/>
       <c r="E43" s="36" t="s">
@@ -10425,7 +10413,7 @@
       <c r="K43" s="36"/>
       <c r="L43" s="36"/>
     </row>
-    <row r="44" spans="1:13" ht="29">
+    <row r="44" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="C44" s="37"/>
       <c r="D44" s="43"/>
       <c r="E44" s="36" t="s">
@@ -10446,7 +10434,7 @@
       <c r="L44" s="36"/>
       <c r="M44" s="37"/>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B45" s="69"/>
       <c r="C45" s="102"/>
       <c r="D45" s="103"/>
@@ -10460,7 +10448,7 @@
       <c r="L45" s="107"/>
       <c r="M45" s="102"/>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="14" t="s">
         <v>632</v>
       </c>
@@ -10485,7 +10473,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C47" s="41"/>
       <c r="D47" s="42"/>
       <c r="E47" s="36" t="s">
@@ -10504,7 +10492,7 @@
       <c r="J47" s="37"/>
       <c r="K47" s="36"/>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C48" s="37"/>
       <c r="D48" s="43"/>
       <c r="E48" s="36" t="s">
@@ -10524,7 +10512,7 @@
       <c r="K48" s="36"/>
       <c r="L48" s="36"/>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B49" s="69"/>
       <c r="C49" s="102"/>
       <c r="D49" s="103"/>
@@ -10538,7 +10526,7 @@
       <c r="L49" s="107"/>
       <c r="M49" s="102"/>
     </row>
-    <row r="50" spans="1:13" ht="43.5">
+    <row r="50" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
         <v>667</v>
       </c>
@@ -10569,9 +10557,9 @@
       <c r="L50" s="160"/>
       <c r="M50" s="161"/>
     </row>
-    <row r="51" spans="1:13" s="14" customFormat="1">
+    <row r="51" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="14" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="B51" s="53">
         <v>3</v>
@@ -10594,7 +10582,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C52" s="37"/>
       <c r="D52" s="43"/>
       <c r="E52" s="36" t="s">
@@ -10615,7 +10603,7 @@
       <c r="L52" s="36"/>
       <c r="M52" s="37"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C53" s="37"/>
       <c r="D53" s="43"/>
       <c r="E53" s="36" t="s">
@@ -10636,7 +10624,7 @@
       <c r="L53" s="36"/>
       <c r="M53" s="37"/>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C54" s="37"/>
       <c r="D54" s="43"/>
       <c r="E54" s="36" t="s">
@@ -10657,7 +10645,7 @@
       <c r="L54" s="36"/>
       <c r="M54" s="37"/>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C55" s="37"/>
       <c r="D55" s="43"/>
       <c r="E55" s="36" t="s">
@@ -10678,7 +10666,7 @@
       <c r="L55" s="36"/>
       <c r="M55" s="37"/>
     </row>
-    <row r="56" spans="1:13" s="188" customFormat="1">
+    <row r="56" spans="1:13" s="188" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B56" s="171"/>
       <c r="C56" s="172"/>
       <c r="D56" s="173"/>
@@ -10700,7 +10688,7 @@
       <c r="L56" s="174"/>
       <c r="M56" s="172"/>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B57" s="167"/>
       <c r="C57" s="185"/>
       <c r="D57" s="186"/>
@@ -10725,11 +10713,11 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" style="49" bestFit="1" customWidth="1"/>
@@ -10746,12 +10734,12 @@
     <col min="13" max="16384" width="8.81640625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>804</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C1" s="178"/>
       <c r="D1" s="178"/>
@@ -10765,7 +10753,7 @@
       <c r="L1" s="178"/>
       <c r="M1" s="178"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>805</v>
       </c>
@@ -10782,7 +10770,7 @@
       <c r="L2" s="178"/>
       <c r="M2" s="178"/>
     </row>
-    <row r="3" spans="1:13" s="62" customFormat="1" ht="29">
+    <row r="3" spans="1:13" s="62" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -10820,7 +10808,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="58">
+    <row r="4" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -10850,7 +10838,7 @@
       <c r="K4" s="28"/>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>2</v>
       </c>
@@ -10870,7 +10858,7 @@
       <c r="K5" s="54"/>
       <c r="L5" s="55"/>
     </row>
-    <row r="6" spans="1:13" ht="43.5">
+    <row r="6" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B6" s="37"/>
       <c r="C6" s="43"/>
       <c r="D6" s="36" t="s">
@@ -10899,7 +10887,7 @@
       </c>
       <c r="L6" s="37"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="69"/>
       <c r="B7" s="70"/>
       <c r="C7" s="71"/>
@@ -10927,7 +10915,7 @@
       </c>
       <c r="L7" s="70"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="53">
         <v>3</v>
       </c>
@@ -10951,7 +10939,7 @@
       </c>
       <c r="L8" s="55"/>
     </row>
-    <row r="9" spans="1:13" ht="29">
+    <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="37"/>
       <c r="C9" s="43"/>
       <c r="D9" s="36" t="s">
@@ -10978,7 +10966,7 @@
       </c>
       <c r="L9" s="37"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B10" s="37"/>
       <c r="C10" s="43"/>
       <c r="D10" s="36" t="s">
@@ -11003,7 +10991,7 @@
       </c>
       <c r="L10" s="37"/>
     </row>
-    <row r="11" spans="1:13" ht="43.5">
+    <row r="11" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="69"/>
       <c r="B11" s="70"/>
       <c r="C11" s="71"/>
@@ -11027,7 +11015,7 @@
       <c r="K11" s="72"/>
       <c r="L11" s="70"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="53">
         <v>4</v>
       </c>
@@ -11051,7 +11039,7 @@
       </c>
       <c r="L12" s="55"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B13" s="37"/>
       <c r="C13" s="43"/>
       <c r="D13" s="36" t="s">
@@ -11076,7 +11064,7 @@
       </c>
       <c r="L13" s="37"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B14" s="37"/>
       <c r="C14" s="43"/>
       <c r="D14" s="36" t="s">
@@ -11101,7 +11089,7 @@
       </c>
       <c r="L14" s="37"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B15" s="37"/>
       <c r="C15" s="43"/>
       <c r="D15" s="36" t="s">
@@ -11126,7 +11114,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="29">
+    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="37"/>
       <c r="C16" s="43"/>
       <c r="D16" s="36" t="s">
@@ -11153,7 +11141,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="69"/>
       <c r="B17" s="70"/>
       <c r="C17" s="71"/>
@@ -11175,7 +11163,7 @@
       <c r="K17" s="72"/>
       <c r="L17" s="70"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="53">
         <v>5</v>
       </c>
@@ -11199,7 +11187,7 @@
       </c>
       <c r="L18" s="55"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B19" s="37"/>
       <c r="C19" s="43"/>
       <c r="D19" s="36" t="s">
@@ -11224,7 +11212,7 @@
       </c>
       <c r="L19" s="37"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B20" s="37"/>
       <c r="C20" s="43"/>
       <c r="D20" s="36" t="s">
@@ -11249,7 +11237,7 @@
       </c>
       <c r="L20" s="37"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B21" s="37"/>
       <c r="C21" s="43"/>
       <c r="D21" s="36" t="s">
@@ -11274,7 +11262,7 @@
       </c>
       <c r="L21" s="37"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B22" s="37"/>
       <c r="C22" s="43"/>
       <c r="D22" s="36" t="s">
@@ -11299,7 +11287,7 @@
       </c>
       <c r="L22" s="37"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B23" s="37"/>
       <c r="C23" s="43"/>
       <c r="D23" s="36" t="s">
@@ -11324,7 +11312,7 @@
       </c>
       <c r="L23" s="37"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B24" s="37"/>
       <c r="C24" s="43"/>
       <c r="D24" s="36" t="s">
@@ -11349,7 +11337,7 @@
       </c>
       <c r="L24" s="37"/>
     </row>
-    <row r="25" spans="1:12" ht="29">
+    <row r="25" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="69"/>
       <c r="B25" s="70"/>
       <c r="C25" s="71"/>
@@ -11373,7 +11361,7 @@
       <c r="K25" s="72"/>
       <c r="L25" s="70"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="53">
         <v>6</v>
       </c>
@@ -11397,7 +11385,7 @@
       </c>
       <c r="L26" s="55"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B27" s="37"/>
       <c r="C27" s="43"/>
       <c r="D27" s="36">
@@ -11417,7 +11405,7 @@
       <c r="K27" s="36"/>
       <c r="L27" s="37"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B28" s="37"/>
       <c r="C28" s="43"/>
       <c r="D28" s="36">
@@ -11437,7 +11425,7 @@
       <c r="K28" s="36"/>
       <c r="L28" s="37"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B29" s="37"/>
       <c r="C29" s="43"/>
       <c r="D29" s="36">
@@ -11457,7 +11445,7 @@
       <c r="K29" s="36"/>
       <c r="L29" s="37"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B30" s="37"/>
       <c r="C30" s="43"/>
       <c r="D30" s="36">
@@ -11477,7 +11465,7 @@
       <c r="K30" s="36"/>
       <c r="L30" s="37"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B31" s="37"/>
       <c r="C31" s="43"/>
       <c r="D31" s="36">
@@ -11497,7 +11485,7 @@
       <c r="K31" s="36"/>
       <c r="L31" s="37"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B32" s="37"/>
       <c r="C32" s="43"/>
       <c r="D32" s="36">
@@ -11517,7 +11505,7 @@
       <c r="K32" s="36"/>
       <c r="L32" s="37"/>
     </row>
-    <row r="33" spans="1:12" ht="29">
+    <row r="33" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="37"/>
       <c r="C33" s="43"/>
       <c r="D33" s="36">
@@ -11542,7 +11530,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="43.5">
+    <row r="34" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B34" s="37"/>
       <c r="C34" s="43"/>
       <c r="D34" s="36" t="s">
@@ -11567,7 +11555,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="69"/>
       <c r="B35" s="70"/>
       <c r="C35" s="71"/>
@@ -11591,7 +11579,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="53"/>
       <c r="B36" s="78"/>
       <c r="C36" s="79"/>
@@ -11616,11 +11604,11 @@
   <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="99" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.1796875" style="37" bestFit="1" customWidth="1"/>
@@ -11637,7 +11625,7 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="18" customFormat="1">
+    <row r="1" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>804</v>
       </c>
@@ -11648,7 +11636,7 @@
       <c r="I1" s="178"/>
       <c r="J1" s="178"/>
     </row>
-    <row r="2" spans="1:12" s="18" customFormat="1">
+    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>805</v>
       </c>
@@ -11657,7 +11645,7 @@
       <c r="I2" s="178"/>
       <c r="J2" s="178"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -11695,7 +11683,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="30">
         <v>1</v>
       </c>
@@ -11727,7 +11715,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="109">
         <v>2</v>
       </c>
@@ -11749,7 +11737,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>5</v>
       </c>
@@ -11769,7 +11757,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>68</v>
       </c>
@@ -11792,7 +11780,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D8" s="36" t="s">
         <v>4</v>
       </c>
@@ -11812,7 +11800,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D9" s="36" t="s">
         <v>73</v>
       </c>
@@ -11832,7 +11820,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="29">
+    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D10" s="36" t="s">
         <v>3</v>
       </c>
@@ -11855,7 +11843,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="58">
+    <row r="11" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="158"/>
       <c r="B11" s="70"/>
       <c r="C11" s="71"/>
@@ -11885,7 +11873,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="43.5">
+    <row r="12" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="158"/>
       <c r="B12" s="70"/>
       <c r="C12" s="71"/>
@@ -11915,7 +11903,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="109">
         <v>3</v>
       </c>
@@ -11937,7 +11925,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D14" s="36" t="s">
         <v>9</v>
       </c>
@@ -11957,7 +11945,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D15" s="36" t="s">
         <v>59</v>
       </c>
@@ -11977,7 +11965,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="29">
+    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="158"/>
       <c r="B16" s="70"/>
       <c r="C16" s="71"/>
@@ -11999,7 +11987,7 @@
       <c r="K16" s="89"/>
       <c r="L16" s="90"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="109">
         <v>4</v>
       </c>
@@ -12025,7 +12013,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D18" s="36" t="s">
         <v>87</v>
       </c>
@@ -12045,7 +12033,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D19" s="36" t="s">
         <v>14</v>
       </c>
@@ -12062,7 +12050,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D20" s="36" t="s">
         <v>3</v>
       </c>
@@ -12082,7 +12070,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="29">
+    <row r="21" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D21" s="36" t="s">
         <v>34</v>
       </c>
@@ -12102,7 +12090,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D22" s="36" t="s">
         <v>5</v>
       </c>
@@ -12122,7 +12110,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D23" s="36" t="s">
         <v>9</v>
       </c>
@@ -12142,7 +12130,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="43.5">
+    <row r="24" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B24" s="70"/>
       <c r="C24" s="71"/>
       <c r="D24" s="72" t="s">
@@ -12169,7 +12157,7 @@
       </c>
       <c r="L24" s="70"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="99">
         <v>5</v>
       </c>
@@ -12193,7 +12181,7 @@
       </c>
       <c r="L25" s="55"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D26" s="36" t="s">
         <v>4</v>
       </c>
@@ -12213,7 +12201,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D27" s="36" t="s">
         <v>6</v>
       </c>
@@ -12233,7 +12221,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D28" s="36" t="s">
         <v>8</v>
       </c>
@@ -12253,7 +12241,7 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="29">
+    <row r="29" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="158"/>
       <c r="B29" s="70"/>
       <c r="C29" s="71"/>
@@ -12277,7 +12265,7 @@
       <c r="K29" s="72"/>
       <c r="L29" s="70"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="109">
         <v>6</v>
       </c>
@@ -12297,7 +12285,7 @@
       <c r="K30" s="54"/>
       <c r="L30" s="55"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D31" s="36" t="s">
         <v>78</v>
       </c>
@@ -12314,7 +12302,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D32" s="36" t="s">
         <v>87</v>
       </c>
@@ -12331,7 +12319,7 @@
         <v>1322</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="158"/>
       <c r="B33" s="70"/>
       <c r="C33" s="71"/>
@@ -12353,7 +12341,7 @@
       <c r="K33" s="72"/>
       <c r="L33" s="70"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="109">
         <v>7</v>
       </c>
@@ -12377,7 +12365,7 @@
       </c>
       <c r="L34" s="55"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D35" s="36">
         <v>1</v>
       </c>
@@ -12391,7 +12379,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D36" s="36">
         <v>2</v>
       </c>
@@ -12405,7 +12393,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D37" s="36">
         <v>3</v>
       </c>
@@ -12419,7 +12407,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D38" s="36" t="s">
         <v>87</v>
       </c>
@@ -12436,7 +12424,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="158"/>
       <c r="B39" s="70"/>
       <c r="C39" s="71"/>
@@ -12458,7 +12446,7 @@
       <c r="K39" s="72"/>
       <c r="L39" s="70"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="109">
         <v>8</v>
       </c>
@@ -12482,7 +12470,7 @@
       </c>
       <c r="L40" s="55"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D41" s="36">
         <v>1</v>
       </c>
@@ -12496,7 +12484,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D42" s="36">
         <v>2</v>
       </c>
@@ -12510,7 +12498,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D43" s="36">
         <v>3</v>
       </c>
@@ -12524,7 +12512,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="29">
+    <row r="44" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="158"/>
       <c r="B44" s="70"/>
       <c r="C44" s="71"/>
@@ -12546,7 +12534,7 @@
       <c r="K44" s="72"/>
       <c r="L44" s="70"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="109">
         <v>9</v>
       </c>
@@ -12570,7 +12558,7 @@
       </c>
       <c r="L45" s="55"/>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D46" s="36" t="s">
         <v>8</v>
       </c>
@@ -12590,7 +12578,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D47" s="36" t="s">
         <v>4</v>
       </c>
@@ -12610,7 +12598,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="43.5">
+    <row r="48" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="158"/>
       <c r="B48" s="70"/>
       <c r="C48" s="71"/>
@@ -12634,7 +12622,7 @@
       <c r="K48" s="72"/>
       <c r="L48" s="70"/>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="109">
         <v>10</v>
       </c>
@@ -12658,7 +12646,7 @@
       </c>
       <c r="L49" s="55"/>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D50" s="36" t="s">
         <v>11</v>
       </c>
@@ -12675,7 +12663,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D51" s="36" t="s">
         <v>4</v>
       </c>
@@ -12695,7 +12683,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="29">
+    <row r="52" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="158"/>
       <c r="B52" s="70"/>
       <c r="C52" s="71"/>
@@ -12717,7 +12705,7 @@
       <c r="K52" s="72"/>
       <c r="L52" s="70"/>
     </row>
-    <row r="53" spans="1:12" ht="43.5">
+    <row r="53" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="109">
         <v>11</v>
       </c>
@@ -12745,7 +12733,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D54" s="36" t="s">
         <v>9</v>
       </c>
@@ -12765,7 +12753,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="158"/>
       <c r="B55" s="70"/>
       <c r="C55" s="71"/>
@@ -12791,7 +12779,7 @@
       </c>
       <c r="L55" s="70"/>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="109"/>
       <c r="B56" s="55"/>
       <c r="C56" s="61"/>
@@ -12816,11 +12804,11 @@
   <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.1796875" style="37" bestFit="1" customWidth="1"/>
@@ -12837,7 +12825,7 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="18" customFormat="1">
+    <row r="1" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>804</v>
       </c>
@@ -12848,7 +12836,7 @@
       <c r="I1" s="178"/>
       <c r="J1" s="178"/>
     </row>
-    <row r="2" spans="1:12" s="18" customFormat="1">
+    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>805</v>
       </c>
@@ -12856,7 +12844,7 @@
       <c r="I2" s="178"/>
       <c r="J2" s="178"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -12894,7 +12882,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -12926,7 +12914,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>2</v>
       </c>
@@ -12948,7 +12936,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>5</v>
       </c>
@@ -12968,7 +12956,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>68</v>
       </c>
@@ -12991,7 +12979,7 @@
         <v>1329</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D8" s="36" t="s">
         <v>4</v>
       </c>
@@ -13011,7 +12999,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D9" s="36" t="s">
         <v>73</v>
       </c>
@@ -13031,7 +13019,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="29">
+    <row r="10" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D10" s="36" t="s">
         <v>3</v>
       </c>
@@ -13054,7 +13042,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="58">
+    <row r="11" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="69"/>
       <c r="B11" s="70"/>
       <c r="C11" s="71"/>
@@ -13084,7 +13072,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="43.5">
+    <row r="12" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="69"/>
       <c r="B12" s="70"/>
       <c r="C12" s="71"/>
@@ -13114,7 +13102,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="53">
         <v>3</v>
       </c>
@@ -13136,7 +13124,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D14" s="36" t="s">
         <v>9</v>
       </c>
@@ -13156,7 +13144,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D15" s="36" t="s">
         <v>59</v>
       </c>
@@ -13176,7 +13164,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="69"/>
       <c r="B16" s="70"/>
       <c r="C16" s="71"/>
@@ -13198,7 +13186,7 @@
       <c r="K16" s="89"/>
       <c r="L16" s="90"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="53">
         <v>4</v>
       </c>
@@ -13224,7 +13212,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="29">
+    <row r="18" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D18" s="36" t="s">
         <v>87</v>
       </c>
@@ -13247,7 +13235,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="29">
+    <row r="19" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D19" s="36" t="s">
         <v>14</v>
       </c>
@@ -13267,7 +13255,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="29">
+    <row r="20" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D20" s="36" t="s">
         <v>3</v>
       </c>
@@ -13290,7 +13278,7 @@
         <v>1258</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="29">
+    <row r="21" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D21" s="36" t="s">
         <v>34</v>
       </c>
@@ -13310,7 +13298,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="29">
+    <row r="22" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D22" s="36" t="s">
         <v>5</v>
       </c>
@@ -13333,7 +13321,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="29">
+    <row r="23" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D23" s="36" t="s">
         <v>9</v>
       </c>
@@ -13356,7 +13344,7 @@
         <v>1312</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="69"/>
       <c r="B24" s="70"/>
       <c r="C24" s="71"/>
@@ -13382,7 +13370,7 @@
       </c>
       <c r="L24" s="70"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="53">
         <v>5</v>
       </c>
@@ -13406,7 +13394,7 @@
       </c>
       <c r="L25" s="78"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B26" s="49"/>
       <c r="C26" s="50"/>
       <c r="D26" s="36" t="s">
@@ -13431,7 +13419,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B27" s="49"/>
       <c r="C27" s="50"/>
       <c r="D27" s="36" t="s">
@@ -13456,7 +13444,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="69"/>
       <c r="B28" s="102"/>
       <c r="C28" s="103"/>
@@ -13482,7 +13470,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="53">
         <v>6</v>
       </c>
@@ -13506,7 +13494,7 @@
       </c>
       <c r="L29" s="78"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B30" s="49"/>
       <c r="C30" s="50"/>
       <c r="D30" s="36" t="s">
@@ -13531,7 +13519,7 @@
       </c>
       <c r="L30" s="49"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B31" s="49"/>
       <c r="C31" s="50"/>
       <c r="D31" s="36" t="s">
@@ -13556,7 +13544,7 @@
       </c>
       <c r="L31" s="49"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="69"/>
       <c r="B32" s="102"/>
       <c r="C32" s="103"/>
@@ -13580,7 +13568,7 @@
       <c r="K32" s="107"/>
       <c r="L32" s="102"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="53">
         <v>7</v>
       </c>
@@ -13604,7 +13592,7 @@
       </c>
       <c r="L33" s="78"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B34" s="49"/>
       <c r="C34" s="50"/>
       <c r="D34" s="36" t="s">
@@ -13629,7 +13617,7 @@
       </c>
       <c r="L34" s="49"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B35" s="49"/>
       <c r="C35" s="50"/>
       <c r="D35" s="36" t="s">
@@ -13654,7 +13642,7 @@
       </c>
       <c r="L35" s="49"/>
     </row>
-    <row r="36" spans="1:12" ht="29">
+    <row r="36" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="69"/>
       <c r="B36" s="102"/>
       <c r="C36" s="103"/>
@@ -13678,7 +13666,7 @@
       <c r="K36" s="107"/>
       <c r="L36" s="102"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="53">
         <v>8</v>
       </c>
@@ -13702,7 +13690,7 @@
       </c>
       <c r="L37" s="78"/>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B38" s="49"/>
       <c r="C38" s="50"/>
       <c r="D38" s="36" t="s">
@@ -13727,7 +13715,7 @@
       </c>
       <c r="L38" s="49"/>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B39" s="49"/>
       <c r="C39" s="50"/>
       <c r="D39" s="36" t="s">
@@ -13752,7 +13740,7 @@
       </c>
       <c r="L39" s="49"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B40" s="49"/>
       <c r="C40" s="50"/>
       <c r="D40" s="36" t="s">
@@ -13777,7 +13765,7 @@
       </c>
       <c r="L40" s="49"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B41" s="49"/>
       <c r="C41" s="50"/>
       <c r="D41" s="36" t="s">
@@ -13802,7 +13790,7 @@
       </c>
       <c r="L41" s="49"/>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B42" s="49"/>
       <c r="C42" s="50"/>
       <c r="D42" s="36" t="s">
@@ -13827,7 +13815,7 @@
       </c>
       <c r="L42" s="49"/>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B43" s="49"/>
       <c r="C43" s="50"/>
       <c r="D43" s="36" t="s">
@@ -13850,7 +13838,7 @@
       </c>
       <c r="L43" s="49"/>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="69"/>
       <c r="B44" s="102"/>
       <c r="C44" s="103"/>
@@ -13874,7 +13862,7 @@
       <c r="K44" s="107"/>
       <c r="L44" s="102"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="53">
         <v>9</v>
       </c>
@@ -13898,7 +13886,7 @@
       </c>
       <c r="L45" s="78"/>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B46" s="49"/>
       <c r="C46" s="50"/>
       <c r="D46" s="36" t="s">
@@ -13925,7 +13913,7 @@
       </c>
       <c r="L46" s="49"/>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B47" s="49"/>
       <c r="C47" s="50"/>
       <c r="D47" s="36" t="s">
@@ -13952,7 +13940,7 @@
       </c>
       <c r="L47" s="49"/>
     </row>
-    <row r="48" spans="1:12" ht="29">
+    <row r="48" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="69"/>
       <c r="B48" s="102"/>
       <c r="C48" s="103"/>
@@ -13976,7 +13964,7 @@
       <c r="K48" s="107"/>
       <c r="L48" s="102"/>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="53">
         <v>10</v>
       </c>
@@ -14000,7 +13988,7 @@
       </c>
       <c r="L49" s="78"/>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B50" s="49"/>
       <c r="C50" s="50"/>
       <c r="D50" s="36" t="s">
@@ -14027,7 +14015,7 @@
       </c>
       <c r="L50" s="49"/>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B51" s="49"/>
       <c r="C51" s="50"/>
       <c r="D51" s="36" t="s">
@@ -14054,7 +14042,7 @@
       </c>
       <c r="L51" s="49"/>
     </row>
-    <row r="52" spans="1:12" ht="29">
+    <row r="52" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="69"/>
       <c r="B52" s="102"/>
       <c r="C52" s="103"/>
@@ -14078,7 +14066,7 @@
       <c r="K52" s="107"/>
       <c r="L52" s="102"/>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="53">
         <v>11</v>
       </c>
@@ -14102,7 +14090,7 @@
       </c>
       <c r="L53" s="78"/>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B54" s="49"/>
       <c r="C54" s="50"/>
       <c r="D54" s="36" t="s">
@@ -14127,7 +14115,7 @@
       </c>
       <c r="L54" s="49"/>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B55" s="49"/>
       <c r="C55" s="50"/>
       <c r="D55" s="36" t="s">
@@ -14152,7 +14140,7 @@
       </c>
       <c r="L55" s="49"/>
     </row>
-    <row r="56" spans="1:12" ht="29">
+    <row r="56" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="69"/>
       <c r="B56" s="102"/>
       <c r="C56" s="103"/>
@@ -14176,7 +14164,7 @@
       <c r="K56" s="107"/>
       <c r="L56" s="49"/>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="53">
         <v>12</v>
       </c>
@@ -14199,7 +14187,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D58" s="36" t="s">
         <v>4</v>
       </c>
@@ -14222,7 +14210,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="29">
+    <row r="59" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D59" s="36" t="s">
         <v>3</v>
       </c>
@@ -14245,7 +14233,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="29">
+    <row r="60" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D60" s="36" t="s">
         <v>8</v>
       </c>
@@ -14268,7 +14256,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="29">
+    <row r="61" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="69"/>
       <c r="B61" s="70"/>
       <c r="C61" s="71"/>
@@ -14292,7 +14280,7 @@
       <c r="K61" s="72"/>
       <c r="L61" s="70"/>
     </row>
-    <row r="62" spans="1:12" ht="43.5">
+    <row r="62" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A62" s="109">
         <v>13</v>
       </c>
@@ -14320,7 +14308,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="84"/>
       <c r="D63" s="36" t="s">
         <v>9</v>
@@ -14341,7 +14329,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="88"/>
       <c r="B64" s="70"/>
       <c r="C64" s="71"/>
@@ -14367,7 +14355,7 @@
       </c>
       <c r="L64" s="70"/>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="53"/>
       <c r="B65" s="55"/>
       <c r="C65" s="61"/>
@@ -14391,12 +14379,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
@@ -14413,7 +14401,7 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="18" customFormat="1">
+    <row r="1" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>804</v>
       </c>
@@ -14424,7 +14412,7 @@
       <c r="I1" s="178"/>
       <c r="J1" s="178"/>
     </row>
-    <row r="2" spans="1:12" s="18" customFormat="1">
+    <row r="2" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>805</v>
       </c>
@@ -14432,7 +14420,7 @@
       <c r="I2" s="178"/>
       <c r="J2" s="178"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -14470,7 +14458,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="58">
+    <row r="4" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -14502,7 +14490,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>2</v>
       </c>
@@ -14522,7 +14510,7 @@
       <c r="K5" s="54"/>
       <c r="L5" s="55"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>6</v>
       </c>
@@ -14542,7 +14530,7 @@
         <v>1477</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="69"/>
       <c r="B7" s="70"/>
       <c r="C7" s="71"/>
@@ -14566,7 +14554,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="58">
+    <row r="8" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="53">
         <v>3</v>
       </c>
@@ -14594,7 +14582,7 @@
       </c>
       <c r="L8" s="55"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D9" s="36" t="s">
         <v>5</v>
       </c>
@@ -14614,7 +14602,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="69"/>
       <c r="B10" s="70"/>
       <c r="C10" s="71"/>
@@ -14640,7 +14628,7 @@
       </c>
       <c r="L10" s="70"/>
     </row>
-    <row r="11" spans="1:12" s="18" customFormat="1" ht="72">
+    <row r="11" spans="1:12" s="18" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="69"/>
       <c r="B11" s="70"/>
       <c r="C11" s="71"/>
@@ -14654,17 +14642,17 @@
         <v>407</v>
       </c>
       <c r="G11" s="74" t="s">
-        <v>812</v>
+        <v>818</v>
       </c>
       <c r="H11" s="75" t="s">
-        <v>811</v>
+        <v>817</v>
       </c>
       <c r="I11" s="74"/>
       <c r="J11" s="72"/>
       <c r="K11" s="72"/>
       <c r="L11" s="70"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="53">
         <v>4</v>
       </c>
@@ -14688,7 +14676,7 @@
       </c>
       <c r="L12" s="55"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D13" s="36" t="s">
         <v>8</v>
       </c>
@@ -14708,7 +14696,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="69"/>
       <c r="B14" s="70"/>
       <c r="C14" s="71"/>
@@ -14734,7 +14722,7 @@
       </c>
       <c r="L14" s="70"/>
     </row>
-    <row r="15" spans="1:12" s="18" customFormat="1" ht="43.5">
+    <row r="15" spans="1:12" s="18" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="69"/>
       <c r="B15" s="70"/>
       <c r="C15" s="71"/>
@@ -14756,7 +14744,7 @@
       <c r="K15" s="72"/>
       <c r="L15" s="70"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="53">
         <v>5</v>
       </c>
@@ -14780,7 +14768,7 @@
       </c>
       <c r="L16" s="55"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D17" s="36" t="s">
         <v>9</v>
       </c>
@@ -14800,7 +14788,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D18" s="36" t="s">
         <v>10</v>
       </c>
@@ -14820,7 +14808,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D19" s="36" t="s">
         <v>34</v>
       </c>
@@ -14840,7 +14828,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D20" s="36" t="s">
         <v>11</v>
       </c>
@@ -14860,7 +14848,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D21" s="36" t="s">
         <v>12</v>
       </c>
@@ -14880,7 +14868,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="69"/>
       <c r="B22" s="70"/>
       <c r="C22" s="71"/>
@@ -14904,7 +14892,7 @@
       </c>
       <c r="L22" s="70"/>
     </row>
-    <row r="23" spans="1:12" s="18" customFormat="1" ht="43.5">
+    <row r="23" spans="1:12" s="18" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="69"/>
       <c r="B23" s="70"/>
       <c r="C23" s="71"/>
@@ -14928,7 +14916,7 @@
       <c r="K23" s="72"/>
       <c r="L23" s="70"/>
     </row>
-    <row r="24" spans="1:12" ht="58">
+    <row r="24" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="53">
         <v>6</v>
       </c>
@@ -14956,7 +14944,7 @@
       </c>
       <c r="L24" s="55"/>
     </row>
-    <row r="25" spans="1:12" ht="29">
+    <row r="25" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D25" s="36" t="s">
         <v>9</v>
       </c>
@@ -14979,7 +14967,7 @@
         <v>2004</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="58">
+    <row r="26" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="69"/>
       <c r="B26" s="70"/>
       <c r="C26" s="71"/>
@@ -15009,7 +14997,7 @@
       </c>
       <c r="L26" s="70"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="53">
         <v>7</v>
       </c>
@@ -15033,7 +15021,7 @@
       </c>
       <c r="L27" s="55"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D28" s="36" t="s">
         <v>4</v>
       </c>
@@ -15056,7 +15044,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D29" s="36" t="s">
         <v>3</v>
       </c>
@@ -15076,7 +15064,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="69"/>
       <c r="B30" s="70"/>
       <c r="C30" s="71"/>
@@ -15102,7 +15090,7 @@
       </c>
       <c r="L30" s="70"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="53"/>
       <c r="B31" s="55"/>
       <c r="C31" s="61"/>
@@ -15130,7 +15118,7 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="115" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" style="110" bestFit="1" customWidth="1"/>
@@ -15146,7 +15134,7 @@
     <col min="12" max="12" width="23.36328125" style="110" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>804</v>
       </c>
@@ -15164,7 +15152,7 @@
       <c r="K1"/>
       <c r="L1"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>805</v>
       </c>
@@ -15180,7 +15168,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -15218,7 +15206,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="58">
+    <row r="4" spans="1:12" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -15252,7 +15240,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>2</v>
       </c>
@@ -15272,7 +15260,7 @@
       <c r="K5" s="54"/>
       <c r="L5" s="55"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="35"/>
       <c r="B6" s="41"/>
       <c r="C6" s="42"/>
@@ -15300,7 +15288,7 @@
       </c>
       <c r="L6" s="37"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="35"/>
       <c r="B7" s="37"/>
       <c r="C7" s="43"/>
@@ -15330,7 +15318,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="69"/>
       <c r="B8" s="70"/>
       <c r="C8" s="71"/>
@@ -15356,7 +15344,7 @@
       </c>
       <c r="L8" s="70"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="53">
         <v>3</v>
       </c>
@@ -15378,7 +15366,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="35"/>
       <c r="B10" s="41"/>
       <c r="C10" s="42"/>
@@ -15400,7 +15388,7 @@
       <c r="K10" s="36"/>
       <c r="L10" s="49"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="35"/>
       <c r="B11" s="37"/>
       <c r="C11" s="43"/>
@@ -15422,7 +15410,7 @@
       <c r="K11" s="36"/>
       <c r="L11" s="37"/>
     </row>
-    <row r="12" spans="1:12" ht="29">
+    <row r="12" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="69"/>
       <c r="B12" s="70"/>
       <c r="C12" s="71"/>
@@ -15446,7 +15434,7 @@
       <c r="K12" s="89"/>
       <c r="L12" s="90"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="53">
         <v>4</v>
       </c>
@@ -15470,7 +15458,7 @@
       </c>
       <c r="L13" s="55"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="35"/>
       <c r="B14" s="41"/>
       <c r="C14" s="42"/>
@@ -15496,7 +15484,7 @@
       </c>
       <c r="L14" s="37"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="35"/>
       <c r="B15" s="37"/>
       <c r="C15" s="43"/>
@@ -15522,7 +15510,7 @@
       </c>
       <c r="L15" s="37"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="69"/>
       <c r="B16" s="70"/>
       <c r="C16" s="71"/>
@@ -15544,7 +15532,7 @@
       <c r="K16" s="72"/>
       <c r="L16" s="70"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="53">
         <v>5</v>
       </c>
@@ -15568,7 +15556,7 @@
       </c>
       <c r="L17" s="55"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="35"/>
       <c r="B18" s="41"/>
       <c r="C18" s="42"/>
@@ -15596,7 +15584,7 @@
       </c>
       <c r="L18" s="37"/>
     </row>
-    <row r="19" spans="1:12" ht="29">
+    <row r="19" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="69"/>
       <c r="B19" s="70"/>
       <c r="C19" s="71"/>
@@ -15624,7 +15612,7 @@
       </c>
       <c r="L19" s="70"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="53">
         <v>6</v>
       </c>
@@ -15648,7 +15636,7 @@
       </c>
       <c r="L20" s="55"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="35"/>
       <c r="B21" s="41"/>
       <c r="C21" s="42"/>
@@ -15674,7 +15662,7 @@
       </c>
       <c r="L21" s="37"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="35"/>
       <c r="B22" s="37"/>
       <c r="C22" s="43"/>
@@ -15700,7 +15688,7 @@
       </c>
       <c r="L22" s="37"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="35"/>
       <c r="B23" s="37"/>
       <c r="C23" s="43"/>
@@ -15726,7 +15714,7 @@
       </c>
       <c r="L23" s="37"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="35"/>
       <c r="B24" s="37"/>
       <c r="C24" s="43"/>
@@ -15752,7 +15740,7 @@
       </c>
       <c r="L24" s="37"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="35"/>
       <c r="B25" s="37"/>
       <c r="C25" s="43"/>
@@ -15778,7 +15766,7 @@
       </c>
       <c r="L25" s="37"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="35"/>
       <c r="B26" s="37"/>
       <c r="C26" s="43"/>
@@ -15802,7 +15790,7 @@
       </c>
       <c r="L26" s="37"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="69"/>
       <c r="B27" s="70"/>
       <c r="C27" s="71"/>
@@ -15824,7 +15812,7 @@
       <c r="K27" s="72"/>
       <c r="L27" s="70"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="116"/>
       <c r="B28" s="181" t="s">
         <v>806</v>
@@ -15854,7 +15842,7 @@
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1796875" style="37" bestFit="1" customWidth="1"/>
@@ -15871,7 +15859,7 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>804</v>
       </c>
@@ -15889,7 +15877,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>805</v>
       </c>
@@ -15905,7 +15893,7 @@
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -15943,7 +15931,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -15975,7 +15963,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12" ht="29">
+    <row r="5" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>2</v>
       </c>
@@ -15997,7 +15985,7 @@
       <c r="K5" s="54"/>
       <c r="L5" s="55"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6" s="41"/>
       <c r="C6" s="42"/>
       <c r="D6" s="36" t="s">
@@ -16019,7 +16007,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>61</v>
       </c>
@@ -16039,7 +16027,7 @@
         <v>3014</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D8" s="36" t="s">
         <v>8</v>
       </c>
@@ -16059,7 +16047,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D9" s="36" t="s">
         <v>34</v>
       </c>
@@ -16079,7 +16067,7 @@
         <v>1270</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="43.5">
+    <row r="10" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D10" s="36" t="s">
         <v>87</v>
       </c>
@@ -16099,7 +16087,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D11" s="36" t="s">
         <v>174</v>
       </c>
@@ -16119,7 +16107,7 @@
         <v>1321</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D12" s="36" t="s">
         <v>14</v>
       </c>
@@ -16139,7 +16127,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="69"/>
       <c r="B13" s="70"/>
       <c r="C13" s="71"/>
@@ -16165,7 +16153,7 @@
       </c>
       <c r="L13" s="70"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="53">
         <v>3</v>
       </c>
@@ -16189,7 +16177,7 @@
       </c>
       <c r="L14" s="55"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D15" s="36">
         <v>1</v>
       </c>
@@ -16209,7 +16197,7 @@
         <v>1288</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D16" s="36">
         <v>2</v>
       </c>
@@ -16229,7 +16217,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D17" s="36">
         <v>3</v>
       </c>
@@ -16252,7 +16240,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="43.5">
+    <row r="18" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="69"/>
       <c r="B18" s="70"/>
       <c r="C18" s="71"/>
@@ -16276,7 +16264,7 @@
       <c r="K18" s="72"/>
       <c r="L18" s="70"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="53">
         <v>4</v>
       </c>
@@ -16300,7 +16288,7 @@
       </c>
       <c r="L19" s="55"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D20" s="36" t="s">
         <v>5</v>
       </c>
@@ -16323,7 +16311,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D21" s="36" t="s">
         <v>6</v>
       </c>
@@ -16346,7 +16334,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="29">
+    <row r="22" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="69"/>
       <c r="B22" s="70"/>
       <c r="C22" s="71"/>
@@ -16370,7 +16358,7 @@
       <c r="K22" s="72"/>
       <c r="L22" s="70"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="53">
         <v>5</v>
       </c>
@@ -16394,7 +16382,7 @@
       </c>
       <c r="L23" s="55"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D24" s="36" t="s">
         <v>8</v>
       </c>
@@ -16414,7 +16402,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="29">
+    <row r="25" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="D25" s="36" t="s">
         <v>4</v>
       </c>
@@ -16437,7 +16425,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="69"/>
       <c r="B26" s="70"/>
       <c r="C26" s="71"/>
@@ -16459,7 +16447,7 @@
       <c r="K26" s="72"/>
       <c r="L26" s="70"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="53">
         <v>6</v>
       </c>
@@ -16483,7 +16471,7 @@
       </c>
       <c r="L27" s="55"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D28" s="36" t="s">
         <v>9</v>
       </c>
@@ -16503,7 +16491,7 @@
         <v>1331</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D29" s="36" t="s">
         <v>10</v>
       </c>
@@ -16523,7 +16511,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D30" s="36" t="s">
         <v>34</v>
       </c>
@@ -16543,7 +16531,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D31" s="36" t="s">
         <v>11</v>
       </c>
@@ -16563,7 +16551,7 @@
         <v>1226</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="69"/>
       <c r="B32" s="70"/>
       <c r="C32" s="71"/>
@@ -16589,7 +16577,7 @@
       </c>
       <c r="L32" s="70"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="53">
         <v>7</v>
       </c>
@@ -16613,7 +16601,7 @@
       </c>
       <c r="L33" s="55"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D34" s="36" t="s">
         <v>9</v>
       </c>
@@ -16633,7 +16621,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="29">
+    <row r="35" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="69"/>
       <c r="B35" s="70"/>
       <c r="C35" s="71"/>
@@ -16663,7 +16651,7 @@
       </c>
       <c r="L35" s="70"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="53"/>
       <c r="B36" s="55"/>
       <c r="C36" s="61"/>
@@ -16691,7 +16679,7 @@
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.453125" style="37" bestFit="1" customWidth="1"/>
@@ -16708,12 +16696,12 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>804</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -16726,7 +16714,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>805</v>
       </c>
@@ -16742,7 +16730,7 @@
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="63" t="s">
         <v>393</v>
       </c>
@@ -16780,7 +16768,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="72.5">
+    <row r="4" spans="1:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -16812,7 +16800,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>2</v>
       </c>
@@ -16832,7 +16820,7 @@
       <c r="K5" s="54"/>
       <c r="L5" s="55"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>4</v>
       </c>
@@ -16852,7 +16840,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D7" s="36" t="s">
         <v>3</v>
       </c>
@@ -16872,7 +16860,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D8" s="36" t="s">
         <v>8</v>
       </c>
@@ -16892,7 +16880,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="69"/>
       <c r="B9" s="70"/>
       <c r="C9" s="71"/>
@@ -16916,7 +16904,7 @@
       <c r="K9" s="72"/>
       <c r="L9" s="70"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="53">
         <v>3</v>
       </c>
@@ -16936,7 +16924,7 @@
       <c r="K10" s="54"/>
       <c r="L10" s="55"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D11" s="36" t="s">
         <v>59</v>
       </c>
@@ -16956,7 +16944,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="176" customFormat="1">
+    <row r="12" spans="1:12" s="176" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="171"/>
       <c r="B12" s="172"/>
       <c r="C12" s="173"/>
@@ -16978,7 +16966,7 @@
       <c r="K12" s="174"/>
       <c r="L12" s="172"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="167"/>
       <c r="B13" s="168"/>
       <c r="C13" s="169"/>
@@ -17007,7 +16995,7 @@
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.81640625" style="37" bestFit="1" customWidth="1"/>
@@ -17024,7 +17012,7 @@
     <col min="13" max="16384" width="8.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>804</v>
       </c>
@@ -17040,7 +17028,7 @@
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>805</v>
       </c>
@@ -17056,7 +17044,7 @@
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
     </row>
-    <row r="3" spans="1:12" s="83" customFormat="1" ht="29">
+    <row r="3" spans="1:12" s="83" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="122" t="s">
         <v>393</v>
       </c>
@@ -17094,7 +17082,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="27">
         <v>1</v>
       </c>
@@ -17126,7 +17114,7 @@
       </c>
       <c r="L4" s="22"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="53">
         <v>2</v>
       </c>
@@ -17150,7 +17138,7 @@
       </c>
       <c r="L5" s="55"/>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D6" s="36" t="s">
         <v>4</v>
       </c>
@@ -17170,7 +17158,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="69"/>
       <c r="B7" s="70"/>
       <c r="C7" s="71"/>
@@ -17196,7 +17184,7 @@
       </c>
       <c r="L7" s="70"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="53">
         <v>3</v>
       </c>
@@ -17220,7 +17208,7 @@
       </c>
       <c r="L8" s="55"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D9" s="36" t="s">
         <v>8</v>
       </c>
@@ -17243,7 +17231,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D10" s="36" t="s">
         <v>4</v>
       </c>
@@ -17266,7 +17254,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="29">
+    <row r="11" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="69"/>
       <c r="B11" s="70"/>
       <c r="C11" s="71"/>
@@ -17290,7 +17278,7 @@
       <c r="K11" s="72"/>
       <c r="L11" s="70"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="53">
         <v>4</v>
       </c>
@@ -17316,7 +17304,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="43.5">
+    <row r="13" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="D13" s="36" t="s">
         <v>10</v>
       </c>
@@ -17333,7 +17321,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D14" s="36" t="s">
         <v>34</v>
       </c>
@@ -17350,7 +17338,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="D15" s="36" t="s">
         <v>11</v>
       </c>
@@ -17364,7 +17352,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="29">
+    <row r="16" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="69"/>
       <c r="B16" s="70"/>
       <c r="C16" s="71"/>
@@ -17388,7 +17376,7 @@
       <c r="K16" s="72"/>
       <c r="L16" s="70"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="53"/>
       <c r="B17" s="55"/>
       <c r="C17" s="61"/>

</xml_diff>